<commit_message>
simplify some code on the training
</commit_message>
<xml_diff>
--- a/semi_seg/runs/cedar/0425_mmwhs/summary_mmwhs.xlsx
+++ b/semi_seg/runs/cedar/0425_mmwhs/summary_mmwhs.xlsx
@@ -4,25 +4,29 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="9138" windowHeight="13094" activeTab="2"/>
+    <workbookView windowWidth="9138" windowHeight="13094" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="summary_mmwhs" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet1" sheetId="3" r:id="rId2"/>
-    <sheet name="整理好的" sheetId="2" r:id="rId3"/>
+    <sheet name="Sheet2" sheetId="4" r:id="rId3"/>
+    <sheet name="Sheet3" sheetId="5" r:id="rId4"/>
+    <sheet name="Sheet4" sheetId="6" r:id="rId5"/>
+    <sheet name="Sheet5" sheetId="7" r:id="rId6"/>
+    <sheet name="整理好的" sheetId="2" r:id="rId7"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">整理好的!$B$1:$J$753</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="6" hidden="1">整理好的!$B$1:$J$753</definedName>
   </definedNames>
   <calcPr calcId="144525"/>
   <pivotCaches>
-    <pivotCache cacheId="0" r:id="rId4"/>
+    <pivotCache cacheId="0" r:id="rId8"/>
   </pivotCaches>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14502" uniqueCount="816">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14608" uniqueCount="816">
   <si>
     <t>feature_0</t>
   </si>
@@ -2477,10 +2481,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
+    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
   <fonts count="20">
     <font>
@@ -2491,16 +2495,9 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
+      <color rgb="FFFFFFFF"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -2515,7 +2512,90 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -2536,46 +2616,9 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -2589,47 +2632,8 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="11"/>
       <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -2656,19 +2660,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
+        <fgColor rgb="FFA5A5A5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
+        <fgColor theme="5" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
+        <fgColor theme="5" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -2680,25 +2684,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="6" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
+        <fgColor theme="8" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
+        <fgColor rgb="FFF2F2F2"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -2716,7 +2714,25 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -2728,19 +2744,37 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="4" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
+        <fgColor theme="8"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5"/>
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -2752,7 +2786,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -2764,13 +2804,25 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
+        <fgColor theme="7"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7"/>
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -2782,61 +2834,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="7" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
+        <fgColor theme="8" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -2847,6 +2851,39 @@
       <right/>
       <top/>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -2865,16 +2902,16 @@
       <diagonal/>
     </border>
     <border>
-      <left style="double">
+      <left style="thin">
         <color rgb="FF3F3F3F"/>
       </left>
-      <right style="double">
+      <right style="thin">
         <color rgb="FF3F3F3F"/>
       </right>
-      <top style="double">
+      <top style="thin">
         <color rgb="FF3F3F3F"/>
       </top>
-      <bottom style="double">
+      <bottom style="thin">
         <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
@@ -2900,30 +2937,6 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="thin">
         <color rgb="FF7F7F7F"/>
       </left>
@@ -2938,166 +2951,157 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="17" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="10" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="24" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="32" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="10" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="17" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="8" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -3120,9 +3124,6 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
@@ -19137,6 +19138,78 @@
 </table>
 </file>
 
+<file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="A1:I3" totalsRowShown="0">
+  <autoFilter ref="A1:I3"/>
+  <tableColumns count="9">
+    <tableColumn id="1" name="feature_0"/>
+    <tableColumn id="2" name="feature_2"/>
+    <tableColumn id="3" name="feature_3"/>
+    <tableColumn id="4" name="feature_4"/>
+    <tableColumn id="5" name="feature_5"/>
+    <tableColumn id="6" name="feature_6"/>
+    <tableColumn id="7" name="feature_9"/>
+    <tableColumn id="8" name="val_dice_DSC_mean"/>
+    <tableColumn id="9" name="test_dice_DSC_mean"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Table3" displayName="Table3" ref="A1:I4" totalsRowShown="0">
+  <autoFilter ref="A1:I4"/>
+  <tableColumns count="9">
+    <tableColumn id="1" name="feature_0"/>
+    <tableColumn id="2" name="feature_2"/>
+    <tableColumn id="3" name="feature_3"/>
+    <tableColumn id="4" name="feature_4"/>
+    <tableColumn id="5" name="feature_5"/>
+    <tableColumn id="6" name="feature_6"/>
+    <tableColumn id="7" name="feature_9"/>
+    <tableColumn id="8" name="val_dice_DSC_mean"/>
+    <tableColumn id="9" name="test_dice_DSC_mean"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="Table4" displayName="Table4" ref="A1:I4" totalsRowShown="0">
+  <autoFilter ref="A1:I4"/>
+  <tableColumns count="9">
+    <tableColumn id="1" name="feature_0"/>
+    <tableColumn id="2" name="feature_2"/>
+    <tableColumn id="3" name="feature_3"/>
+    <tableColumn id="4" name="feature_4"/>
+    <tableColumn id="5" name="feature_5"/>
+    <tableColumn id="6" name="feature_6"/>
+    <tableColumn id="7" name="feature_9"/>
+    <tableColumn id="8" name="val_dice_DSC_mean"/>
+    <tableColumn id="9" name="test_dice_DSC_mean"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="Table5" displayName="Table5" ref="A1:I3" totalsRowShown="0">
+  <autoFilter ref="A1:I3"/>
+  <tableColumns count="9">
+    <tableColumn id="1" name="feature_0"/>
+    <tableColumn id="2" name="feature_2"/>
+    <tableColumn id="3" name="feature_3"/>
+    <tableColumn id="4" name="feature_4"/>
+    <tableColumn id="5" name="feature_5"/>
+    <tableColumn id="6" name="feature_6"/>
+    <tableColumn id="7" name="feature_9"/>
+    <tableColumn id="8" name="val_dice_DSC_mean"/>
+    <tableColumn id="9" name="test_dice_DSC_mean"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office">
   <a:themeElements>
@@ -50246,10 +50319,508 @@
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
+  <dimension ref="A1:I3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1:I3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="8.99212598425197" defaultRowHeight="14.2" outlineLevelRow="2"/>
+  <cols>
+    <col min="8" max="9" width="12.503937007874"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D1" t="s">
+        <v>4</v>
+      </c>
+      <c r="E1" t="s">
+        <v>5</v>
+      </c>
+      <c r="F1" t="s">
+        <v>6</v>
+      </c>
+      <c r="G1" t="s">
+        <v>9</v>
+      </c>
+      <c r="H1" t="s">
+        <v>10</v>
+      </c>
+      <c r="I1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9">
+      <c r="A2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B2" t="s">
+        <v>25</v>
+      </c>
+      <c r="C2" t="s">
+        <v>190</v>
+      </c>
+      <c r="D2" t="s">
+        <v>32</v>
+      </c>
+      <c r="E2" t="s">
+        <v>33</v>
+      </c>
+      <c r="F2" t="s">
+        <v>65</v>
+      </c>
+      <c r="G2" t="s">
+        <v>16</v>
+      </c>
+      <c r="H2">
+        <v>0.803146719932556</v>
+      </c>
+      <c r="I2">
+        <v>0.747540493806203</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9">
+      <c r="A3" t="s">
+        <v>565</v>
+      </c>
+      <c r="B3" t="s">
+        <v>25</v>
+      </c>
+      <c r="C3" t="s">
+        <v>190</v>
+      </c>
+      <c r="D3" t="s">
+        <v>32</v>
+      </c>
+      <c r="E3" t="s">
+        <v>33</v>
+      </c>
+      <c r="F3" t="s">
+        <v>65</v>
+      </c>
+      <c r="G3" t="s">
+        <v>16</v>
+      </c>
+      <c r="H3">
+        <v>0.794778128465016</v>
+      </c>
+      <c r="I3">
+        <v>0.724498212337493</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <headerFooter/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
+  <dimension ref="A1:I4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1:I4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="8.93700787401575" defaultRowHeight="14.2" outlineLevelRow="3"/>
+  <cols>
+    <col min="8" max="9" width="12.6220472440945"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D1" t="s">
+        <v>4</v>
+      </c>
+      <c r="E1" t="s">
+        <v>5</v>
+      </c>
+      <c r="F1" t="s">
+        <v>6</v>
+      </c>
+      <c r="G1" t="s">
+        <v>9</v>
+      </c>
+      <c r="H1" t="s">
+        <v>10</v>
+      </c>
+      <c r="I1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9">
+      <c r="A2" t="s">
+        <v>565</v>
+      </c>
+      <c r="B2" t="s">
+        <v>25</v>
+      </c>
+      <c r="C2" t="s">
+        <v>26</v>
+      </c>
+      <c r="D2" t="s">
+        <v>32</v>
+      </c>
+      <c r="E2" t="s">
+        <v>33</v>
+      </c>
+      <c r="F2" t="s">
+        <v>130</v>
+      </c>
+      <c r="G2" t="s">
+        <v>18</v>
+      </c>
+      <c r="H2">
+        <v>0.370917538801829</v>
+      </c>
+      <c r="I2">
+        <v>0.510018448034922</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9">
+      <c r="A3" t="s">
+        <v>13</v>
+      </c>
+      <c r="B3" t="s">
+        <v>25</v>
+      </c>
+      <c r="C3" t="s">
+        <v>26</v>
+      </c>
+      <c r="D3" t="s">
+        <v>32</v>
+      </c>
+      <c r="E3" t="s">
+        <v>33</v>
+      </c>
+      <c r="F3" t="s">
+        <v>130</v>
+      </c>
+      <c r="G3" t="s">
+        <v>18</v>
+      </c>
+      <c r="H3">
+        <v>0.367546007037162</v>
+      </c>
+      <c r="I3">
+        <v>0.482491513093312</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9">
+      <c r="A4" t="s">
+        <v>312</v>
+      </c>
+      <c r="B4" t="s">
+        <v>25</v>
+      </c>
+      <c r="C4" t="s">
+        <v>26</v>
+      </c>
+      <c r="D4" t="s">
+        <v>32</v>
+      </c>
+      <c r="E4" t="s">
+        <v>33</v>
+      </c>
+      <c r="F4" t="s">
+        <v>130</v>
+      </c>
+      <c r="G4" t="s">
+        <v>18</v>
+      </c>
+      <c r="H4">
+        <v>0.360126286745071</v>
+      </c>
+      <c r="I4">
+        <v>0.467077374458313</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <headerFooter/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
+  <dimension ref="A1:I4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1:I4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="8.93700787401575" defaultRowHeight="14.2" outlineLevelRow="3"/>
+  <cols>
+    <col min="8" max="9" width="12.6220472440945"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D1" t="s">
+        <v>4</v>
+      </c>
+      <c r="E1" t="s">
+        <v>5</v>
+      </c>
+      <c r="F1" t="s">
+        <v>6</v>
+      </c>
+      <c r="G1" t="s">
+        <v>9</v>
+      </c>
+      <c r="H1" t="s">
+        <v>10</v>
+      </c>
+      <c r="I1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9">
+      <c r="A2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B2" t="s">
+        <v>25</v>
+      </c>
+      <c r="C2" t="s">
+        <v>190</v>
+      </c>
+      <c r="D2" t="s">
+        <v>27</v>
+      </c>
+      <c r="E2" t="s">
+        <v>27</v>
+      </c>
+      <c r="F2" t="s">
+        <v>27</v>
+      </c>
+      <c r="G2" t="s">
+        <v>18</v>
+      </c>
+      <c r="H2">
+        <v>0.330980598926544</v>
+      </c>
+      <c r="I2">
+        <v>0.508267611265182</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9">
+      <c r="A3" t="s">
+        <v>312</v>
+      </c>
+      <c r="B3" t="s">
+        <v>25</v>
+      </c>
+      <c r="C3" t="s">
+        <v>190</v>
+      </c>
+      <c r="D3" t="s">
+        <v>27</v>
+      </c>
+      <c r="E3" t="s">
+        <v>27</v>
+      </c>
+      <c r="F3" t="s">
+        <v>27</v>
+      </c>
+      <c r="G3" t="s">
+        <v>18</v>
+      </c>
+      <c r="H3">
+        <v>0.368343621492385</v>
+      </c>
+      <c r="I3">
+        <v>0.466466834147771</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9">
+      <c r="A4" t="s">
+        <v>565</v>
+      </c>
+      <c r="B4" t="s">
+        <v>25</v>
+      </c>
+      <c r="C4" t="s">
+        <v>190</v>
+      </c>
+      <c r="D4" t="s">
+        <v>27</v>
+      </c>
+      <c r="E4" t="s">
+        <v>27</v>
+      </c>
+      <c r="F4" t="s">
+        <v>27</v>
+      </c>
+      <c r="G4" t="s">
+        <v>18</v>
+      </c>
+      <c r="H4">
+        <v>0.328365912040074</v>
+      </c>
+      <c r="I4">
+        <v>0.372259025772412</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <headerFooter/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
+  <dimension ref="A1:I3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1:I3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="8.93700787401575" defaultRowHeight="14.2" outlineLevelRow="2"/>
+  <cols>
+    <col min="8" max="9" width="12.6220472440945"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D1" t="s">
+        <v>4</v>
+      </c>
+      <c r="E1" t="s">
+        <v>5</v>
+      </c>
+      <c r="F1" t="s">
+        <v>6</v>
+      </c>
+      <c r="G1" t="s">
+        <v>9</v>
+      </c>
+      <c r="H1" t="s">
+        <v>10</v>
+      </c>
+      <c r="I1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9">
+      <c r="A2" t="s">
+        <v>565</v>
+      </c>
+      <c r="B2" t="s">
+        <v>25</v>
+      </c>
+      <c r="C2" t="s">
+        <v>190</v>
+      </c>
+      <c r="D2" t="s">
+        <v>32</v>
+      </c>
+      <c r="E2" t="s">
+        <v>33</v>
+      </c>
+      <c r="F2" t="s">
+        <v>65</v>
+      </c>
+      <c r="G2" t="s">
+        <v>18</v>
+      </c>
+      <c r="H2">
+        <v>0.293486619989077</v>
+      </c>
+      <c r="I2">
+        <v>0.468035866816838</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9">
+      <c r="A3" t="s">
+        <v>13</v>
+      </c>
+      <c r="B3" t="s">
+        <v>25</v>
+      </c>
+      <c r="C3" t="s">
+        <v>190</v>
+      </c>
+      <c r="D3" t="s">
+        <v>32</v>
+      </c>
+      <c r="E3" t="s">
+        <v>33</v>
+      </c>
+      <c r="F3" t="s">
+        <v>65</v>
+      </c>
+      <c r="G3" t="s">
+        <v>18</v>
+      </c>
+      <c r="H3">
+        <v>0.349817608793576</v>
+      </c>
+      <c r="I3">
+        <v>0.432661712169647</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <headerFooter/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
   <dimension ref="A1:X753"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" topLeftCell="J37" workbookViewId="0">
-      <selection activeCell="P43" sqref="P43"/>
+    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" topLeftCell="J7" workbookViewId="0">
+      <selection activeCell="L41" sqref="L41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.50393700787402" defaultRowHeight="14.2"/>
@@ -50494,16 +51065,16 @@
       <c r="S5" t="s">
         <v>14</v>
       </c>
-      <c r="U5" s="9">
+      <c r="U5" s="8">
         <v>0.0354104661996715</v>
       </c>
-      <c r="V5" s="9">
+      <c r="V5" s="8">
         <v>0.0339710225484447</v>
       </c>
-      <c r="W5" s="9">
+      <c r="W5" s="8">
         <v>0.0243002439600468</v>
       </c>
-      <c r="X5" s="9">
+      <c r="X5" s="8">
         <v>0.143969757051101</v>
       </c>
     </row>
@@ -50556,16 +51127,16 @@
       <c r="T6" t="s">
         <v>14</v>
       </c>
-      <c r="U6" s="9">
+      <c r="U6" s="8">
         <v>0.0354104661996715</v>
       </c>
-      <c r="V6" s="9">
+      <c r="V6" s="8">
         <v>0.0339710225484447</v>
       </c>
-      <c r="W6" s="9">
+      <c r="W6" s="8">
         <v>0.0243002439600468</v>
       </c>
-      <c r="X6" s="9">
+      <c r="X6" s="8">
         <v>0.143969757051101</v>
       </c>
     </row>
@@ -50618,16 +51189,16 @@
       <c r="S7" t="s">
         <v>26</v>
       </c>
-      <c r="U7" s="9">
+      <c r="U7" s="8">
         <v>0.0503600988014527</v>
       </c>
-      <c r="V7" s="9">
+      <c r="V7" s="8">
         <v>0.0420038694377381</v>
       </c>
-      <c r="W7" s="9">
+      <c r="W7" s="8">
         <v>0.0140957158512121</v>
       </c>
-      <c r="X7" s="9">
+      <c r="X7" s="8">
         <v>0.12592184037788</v>
       </c>
     </row>
@@ -50680,16 +51251,16 @@
       <c r="T8" t="s">
         <v>27</v>
       </c>
-      <c r="U8" s="9">
+      <c r="U8" s="8">
         <v>0.0416421572380358</v>
       </c>
-      <c r="V8" s="9">
+      <c r="V8" s="8">
         <v>0.00409812095707825</v>
       </c>
-      <c r="W8" s="9">
+      <c r="W8" s="8">
         <v>0.00835008628381544</v>
       </c>
-      <c r="X8" s="9">
+      <c r="X8" s="8">
         <v>0.12764199486513</v>
       </c>
     </row>
@@ -50739,19 +51310,19 @@
       <c r="Q9" s="4">
         <v>0.599029784401257</v>
       </c>
-      <c r="T9" s="8" t="s">
+      <c r="T9" s="3" t="s">
         <v>65</v>
       </c>
-      <c r="U9" s="10">
+      <c r="U9" s="9">
         <v>0.0356617226800387</v>
       </c>
-      <c r="V9" s="10">
+      <c r="V9" s="9">
         <v>0.017191021432642</v>
       </c>
-      <c r="W9" s="10">
+      <c r="W9" s="9">
         <v>0.00656696310907832</v>
       </c>
-      <c r="X9" s="10">
+      <c r="X9" s="9">
         <v>0.127203963720594</v>
       </c>
     </row>
@@ -50804,16 +51375,16 @@
       <c r="T10" t="s">
         <v>110</v>
       </c>
-      <c r="U10" s="9">
+      <c r="U10" s="8">
         <v>0.0320816971965958</v>
       </c>
-      <c r="V10" s="9">
+      <c r="V10" s="8">
         <v>0.0360178822756663</v>
       </c>
-      <c r="W10" s="9">
+      <c r="W10" s="8">
         <v>0.00750285166592939</v>
       </c>
-      <c r="X10" s="9">
+      <c r="X10" s="8">
         <v>0.121240809868784</v>
       </c>
     </row>
@@ -50866,16 +51437,16 @@
       <c r="T11" t="s">
         <v>50</v>
       </c>
-      <c r="U11" s="9">
+      <c r="U11" s="8">
         <v>0.0317033437405383</v>
       </c>
-      <c r="V11" s="9">
+      <c r="V11" s="8">
         <v>0.0530358378313302</v>
       </c>
-      <c r="W11" s="9">
+      <c r="W11" s="8">
         <v>0.0208618114746544</v>
       </c>
-      <c r="X11" s="9">
+      <c r="X11" s="8">
         <v>0.144314374924082</v>
       </c>
     </row>
@@ -50928,16 +51499,16 @@
       <c r="T12" t="s">
         <v>100</v>
       </c>
-      <c r="U12" s="9">
+      <c r="U12" s="8">
         <v>0.0626186649331548</v>
       </c>
-      <c r="V12" s="9">
+      <c r="V12" s="8">
         <v>0.0436272317507562</v>
       </c>
-      <c r="W12" s="9">
+      <c r="W12" s="8">
         <v>0.00647679249963594</v>
       </c>
-      <c r="X12" s="9">
+      <c r="X12" s="8">
         <v>0.124067823140757</v>
       </c>
     </row>
@@ -50990,16 +51561,16 @@
       <c r="T13" t="s">
         <v>279</v>
       </c>
-      <c r="U13" s="9">
+      <c r="U13" s="8">
         <v>0.0509188336630661</v>
       </c>
-      <c r="V13" s="9">
+      <c r="V13" s="8">
         <v>0.0106526017189026</v>
       </c>
-      <c r="W13" s="9">
+      <c r="W13" s="8">
         <v>0.0075591504573822</v>
       </c>
-      <c r="X13" s="9">
+      <c r="X13" s="8">
         <v>0.162575096898132</v>
       </c>
     </row>
@@ -51052,16 +51623,16 @@
       <c r="T14" s="5" t="s">
         <v>130</v>
       </c>
-      <c r="U14" s="11">
+      <c r="U14" s="10">
         <v>0.0177615803133576</v>
       </c>
-      <c r="V14" s="11">
+      <c r="V14" s="10">
         <v>0.0365516814026041</v>
       </c>
-      <c r="W14" s="11">
+      <c r="W14" s="10">
         <v>0.00879225839038402</v>
       </c>
-      <c r="X14" s="11">
+      <c r="X14" s="10">
         <v>0.103504130460641</v>
       </c>
     </row>
@@ -51114,16 +51685,16 @@
       <c r="T15" t="s">
         <v>160</v>
       </c>
-      <c r="U15" s="9">
+      <c r="U15" s="8">
         <v>0.046328675385246</v>
       </c>
-      <c r="V15" s="9">
+      <c r="V15" s="8">
         <v>0.0248448896642922</v>
       </c>
-      <c r="W15" s="9">
+      <c r="W15" s="8">
         <v>0.00380441416096851</v>
       </c>
-      <c r="X15" s="9">
+      <c r="X15" s="8">
         <v>0.105353230094429</v>
       </c>
     </row>
@@ -51176,16 +51747,16 @@
       <c r="T16" t="s">
         <v>165</v>
       </c>
-      <c r="U16" s="9">
+      <c r="U16" s="8">
         <v>0.0104802350203184</v>
       </c>
-      <c r="V16" s="9">
+      <c r="V16" s="8">
         <v>0.00194166103996279</v>
       </c>
-      <c r="W16" s="9">
+      <c r="W16" s="8">
         <v>0.00211403767268155</v>
       </c>
-      <c r="X16" s="9">
+      <c r="X16" s="8">
         <v>0.111838596638883</v>
       </c>
     </row>
@@ -51238,16 +51809,16 @@
       <c r="T17" t="s">
         <v>175</v>
       </c>
-      <c r="U17" s="9">
+      <c r="U17" s="8">
         <v>0.0236240548291519</v>
       </c>
-      <c r="V17" s="9">
+      <c r="V17" s="8">
         <v>0.0314050557770129</v>
       </c>
-      <c r="W17" s="9">
+      <c r="W17" s="8">
         <v>0.00691378969363775</v>
       </c>
-      <c r="X17" s="9">
+      <c r="X17" s="8">
         <v>0.150351296371913</v>
       </c>
     </row>
@@ -51300,16 +51871,16 @@
       <c r="T18" t="s">
         <v>180</v>
       </c>
-      <c r="U18" s="9">
+      <c r="U18" s="8">
         <v>0.0251987299513517</v>
       </c>
-      <c r="V18" s="9">
+      <c r="V18" s="8">
         <v>0.0184503262338229</v>
       </c>
-      <c r="W18" s="9">
+      <c r="W18" s="8">
         <v>0.00432160142771029</v>
       </c>
-      <c r="X18" s="9">
+      <c r="X18" s="8">
         <v>0.128810691065415</v>
       </c>
     </row>
@@ -51362,16 +51933,16 @@
       <c r="T19" t="s">
         <v>155</v>
       </c>
-      <c r="U19" s="9">
+      <c r="U19" s="8">
         <v>0.0245948970164859</v>
       </c>
-      <c r="V19" s="9">
+      <c r="V19" s="8">
         <v>0.0356345544085508</v>
       </c>
-      <c r="W19" s="9">
+      <c r="W19" s="8">
         <v>0.015508450320854</v>
       </c>
-      <c r="X19" s="9">
+      <c r="X19" s="8">
         <v>0.109582853674759</v>
       </c>
     </row>
@@ -51424,16 +51995,16 @@
       <c r="T20" t="s">
         <v>40</v>
       </c>
-      <c r="U20" s="9">
+      <c r="U20" s="8">
         <v>0.0238001518196955</v>
       </c>
-      <c r="V20" s="9">
+      <c r="V20" s="8">
         <v>0.0209401738835648</v>
       </c>
-      <c r="W20" s="9">
+      <c r="W20" s="8">
         <v>0.0167509707165659</v>
       </c>
-      <c r="X20" s="9">
+      <c r="X20" s="8">
         <v>0.112429121160858</v>
       </c>
     </row>
@@ -51486,16 +52057,16 @@
       <c r="T21" t="s">
         <v>140</v>
       </c>
-      <c r="U21" s="9">
+      <c r="U21" s="8">
         <v>0.0582903403971914</v>
       </c>
-      <c r="V21" s="9">
+      <c r="V21" s="8">
         <v>0.0229343441326258</v>
       </c>
-      <c r="W21" s="9">
+      <c r="W21" s="8">
         <v>0.0101335117352407</v>
       </c>
-      <c r="X21" s="9">
+      <c r="X21" s="8">
         <v>0.122891503077222</v>
       </c>
     </row>
@@ -51548,16 +52119,16 @@
       <c r="T22" t="s">
         <v>55</v>
       </c>
-      <c r="U22" s="9">
+      <c r="U22" s="8">
         <v>0.0381519294608377</v>
       </c>
-      <c r="V22" s="9">
+      <c r="V22" s="8">
         <v>0.0437410634348036</v>
       </c>
-      <c r="W22" s="9">
+      <c r="W22" s="8">
         <v>0.00314493356638131</v>
       </c>
-      <c r="X22" s="9">
+      <c r="X22" s="8">
         <v>0.128615899708445</v>
       </c>
     </row>
@@ -51610,16 +52181,16 @@
       <c r="T23" t="s">
         <v>120</v>
       </c>
-      <c r="U23" s="9">
+      <c r="U23" s="8">
         <v>0.041571361210884</v>
       </c>
-      <c r="V23" s="9">
+      <c r="V23" s="8">
         <v>0.0133069424325075</v>
       </c>
-      <c r="W23" s="9">
+      <c r="W23" s="8">
         <v>0.00429744236648946</v>
       </c>
-      <c r="X23" s="9">
+      <c r="X23" s="8">
         <v>0.116294860258601</v>
       </c>
     </row>
@@ -51672,16 +52243,16 @@
       <c r="T24" t="s">
         <v>75</v>
       </c>
-      <c r="U24" s="9">
+      <c r="U24" s="8">
         <v>0.0286475031382726</v>
       </c>
-      <c r="V24" s="9">
+      <c r="V24" s="8">
         <v>0.00633255685159926</v>
       </c>
-      <c r="W24" s="9">
+      <c r="W24" s="8">
         <v>0.0145870476839187</v>
       </c>
-      <c r="X24" s="9">
+      <c r="X24" s="8">
         <v>0.112841307704553</v>
       </c>
     </row>
@@ -51734,16 +52305,16 @@
       <c r="T25" t="s">
         <v>115</v>
       </c>
-      <c r="U25" s="9">
+      <c r="U25" s="8">
         <v>0.0363513273552277</v>
       </c>
-      <c r="V25" s="9">
+      <c r="V25" s="8">
         <v>0.0535877911246415</v>
       </c>
-      <c r="W25" s="9">
+      <c r="W25" s="8">
         <v>0.0103103397438084</v>
       </c>
-      <c r="X25" s="9">
+      <c r="X25" s="8">
         <v>0.133955639924961</v>
       </c>
     </row>
@@ -51796,16 +52367,16 @@
       <c r="T26" t="s">
         <v>45</v>
       </c>
-      <c r="U26" s="9">
+      <c r="U26" s="8">
         <v>0.0698183391185413</v>
       </c>
-      <c r="V26" s="9">
+      <c r="V26" s="8">
         <v>0.0100869440293832</v>
       </c>
-      <c r="W26" s="9">
+      <c r="W26" s="8">
         <v>0.00444316714146029</v>
       </c>
-      <c r="X26" s="9">
+      <c r="X26" s="8">
         <v>0.136431070622543</v>
       </c>
     </row>
@@ -51858,16 +52429,16 @@
       <c r="T27" t="s">
         <v>105</v>
       </c>
-      <c r="U27" s="9">
+      <c r="U27" s="8">
         <v>0.025149426625485</v>
       </c>
-      <c r="V27" s="9">
+      <c r="V27" s="8">
         <v>0.0697263769206726</v>
       </c>
-      <c r="W27" s="9">
+      <c r="W27" s="8">
         <v>0.00726855105015165</v>
       </c>
-      <c r="X27" s="9">
+      <c r="X27" s="8">
         <v>0.140145845419505</v>
       </c>
     </row>
@@ -51920,16 +52491,16 @@
       <c r="T28" t="s">
         <v>170</v>
       </c>
-      <c r="U28" s="9">
+      <c r="U28" s="8">
         <v>0.0093140640519097</v>
       </c>
-      <c r="V28" s="9">
+      <c r="V28" s="8">
         <v>0.00450232088432919</v>
       </c>
-      <c r="W28" s="9">
+      <c r="W28" s="8">
         <v>0.0225935065483857</v>
       </c>
-      <c r="X28" s="9">
+      <c r="X28" s="8">
         <v>0.114121770321577</v>
       </c>
     </row>
@@ -51982,16 +52553,16 @@
       <c r="T29" t="s">
         <v>125</v>
       </c>
-      <c r="U29" s="9">
+      <c r="U29" s="8">
         <v>0.0208532170704754</v>
       </c>
-      <c r="V29" s="9">
+      <c r="V29" s="8">
         <v>0.0378732829106148</v>
       </c>
-      <c r="W29" s="9">
+      <c r="W29" s="8">
         <v>0.0041851486429585</v>
       </c>
-      <c r="X29" s="9">
+      <c r="X29" s="8">
         <v>0.150619769657076</v>
       </c>
     </row>
@@ -52044,16 +52615,16 @@
       <c r="T30" t="s">
         <v>60</v>
       </c>
-      <c r="U30" s="9">
+      <c r="U30" s="8">
         <v>0.0329532871643701</v>
       </c>
-      <c r="V30" s="9">
+      <c r="V30" s="8">
         <v>0.0242667694886524</v>
       </c>
-      <c r="W30" s="9">
+      <c r="W30" s="8">
         <v>0.00794752438863662</v>
       </c>
-      <c r="X30" s="9">
+      <c r="X30" s="8">
         <v>0.120533619602173</v>
       </c>
     </row>
@@ -52106,16 +52677,16 @@
       <c r="T31" t="s">
         <v>80</v>
       </c>
-      <c r="U31" s="9">
+      <c r="U31" s="8">
         <v>0.0336149029606789</v>
       </c>
-      <c r="V31" s="9">
+      <c r="V31" s="8">
         <v>0.03591324262049</v>
       </c>
-      <c r="W31" s="9">
+      <c r="W31" s="8">
         <v>0.00781494911603226</v>
       </c>
-      <c r="X31" s="9">
+      <c r="X31" s="8">
         <v>0.122968412642353</v>
       </c>
     </row>
@@ -52168,16 +52739,16 @@
       <c r="T32" t="s">
         <v>90</v>
       </c>
-      <c r="U32" s="9">
+      <c r="U32" s="8">
         <v>0.0286680212469503</v>
       </c>
-      <c r="V32" s="9">
+      <c r="V32" s="8">
         <v>0.0424674992714413</v>
       </c>
-      <c r="W32" s="9">
+      <c r="W32" s="8">
         <v>0.0107368437014616</v>
       </c>
-      <c r="X32" s="9">
+      <c r="X32" s="8">
         <v>0.121231471394024</v>
       </c>
     </row>
@@ -52230,16 +52801,16 @@
       <c r="T33" t="s">
         <v>135</v>
       </c>
-      <c r="U33" s="9">
+      <c r="U33" s="8">
         <v>0.047031309476517</v>
       </c>
-      <c r="V33" s="9">
+      <c r="V33" s="8">
         <v>0.025712473386082</v>
       </c>
-      <c r="W33" s="9">
+      <c r="W33" s="8">
         <v>0.0124854784244513</v>
       </c>
-      <c r="X33" s="9">
+      <c r="X33" s="8">
         <v>0.108021035054908</v>
       </c>
     </row>
@@ -52292,16 +52863,16 @@
       <c r="T34" t="s">
         <v>85</v>
       </c>
-      <c r="U34" s="9">
+      <c r="U34" s="8">
         <v>0.0522718164873258</v>
       </c>
-      <c r="V34" s="9">
+      <c r="V34" s="8">
         <v>0.0515620306472153</v>
       </c>
-      <c r="W34" s="9">
+      <c r="W34" s="8">
         <v>0.00483246509492367</v>
       </c>
-      <c r="X34" s="9">
+      <c r="X34" s="8">
         <v>0.145683395082366</v>
       </c>
     </row>
@@ -52354,16 +52925,16 @@
       <c r="T35" t="s">
         <v>34</v>
       </c>
-      <c r="U35" s="9">
+      <c r="U35" s="8">
         <v>0.0240670738677079</v>
       </c>
-      <c r="V35" s="9">
+      <c r="V35" s="8">
         <v>0.0376156044778414</v>
       </c>
-      <c r="W35" s="9">
+      <c r="W35" s="8">
         <v>0.0056465301848139</v>
       </c>
-      <c r="X35" s="9">
+      <c r="X35" s="8">
         <v>0.131429574798174</v>
       </c>
     </row>
@@ -52416,16 +52987,16 @@
       <c r="T36" t="s">
         <v>70</v>
       </c>
-      <c r="U36" s="9">
+      <c r="U36" s="8">
         <v>0.0346219608546395</v>
       </c>
-      <c r="V36" s="9">
+      <c r="V36" s="8">
         <v>0.0186994227585946</v>
       </c>
-      <c r="W36" s="9">
+      <c r="W36" s="8">
         <v>0.007230540853357</v>
       </c>
-      <c r="X36" s="9">
+      <c r="X36" s="8">
         <v>0.0970630013219297</v>
       </c>
     </row>
@@ -52478,16 +53049,16 @@
       <c r="T37" t="s">
         <v>145</v>
       </c>
-      <c r="U37" s="9">
+      <c r="U37" s="8">
         <v>0.0610940470351256</v>
       </c>
-      <c r="V37" s="9">
+      <c r="V37" s="8">
         <v>0.0380780988919449</v>
       </c>
-      <c r="W37" s="9">
+      <c r="W37" s="8">
         <v>0.0180464888697084</v>
       </c>
-      <c r="X37" s="9">
+      <c r="X37" s="8">
         <v>0.116767086479315</v>
       </c>
     </row>
@@ -52540,16 +53111,16 @@
       <c r="T38" t="s">
         <v>150</v>
       </c>
-      <c r="U38" s="9">
+      <c r="U38" s="8">
         <v>0.0706499742683392</v>
       </c>
-      <c r="V38" s="9">
+      <c r="V38" s="8">
         <v>0.0990837385678982</v>
       </c>
-      <c r="W38" s="9">
+      <c r="W38" s="8">
         <v>0.0244109354629066</v>
       </c>
-      <c r="X38" s="9">
+      <c r="X38" s="8">
         <v>0.123743001755884</v>
       </c>
     </row>
@@ -52602,16 +53173,16 @@
       <c r="T39" t="s">
         <v>95</v>
       </c>
-      <c r="U39" s="9">
+      <c r="U39" s="8">
         <v>0.0268965357322983</v>
       </c>
-      <c r="V39" s="9">
+      <c r="V39" s="8">
         <v>0.0254490929506302</v>
       </c>
-      <c r="W39" s="9">
+      <c r="W39" s="8">
         <v>0.00255749650161541</v>
       </c>
-      <c r="X39" s="9">
+      <c r="X39" s="8">
         <v>0.116633575228388</v>
       </c>
     </row>
@@ -52664,16 +53235,16 @@
       <c r="T40" t="s">
         <v>185</v>
       </c>
-      <c r="U40" s="9">
+      <c r="U40" s="8">
         <v>0.055471420096411</v>
       </c>
-      <c r="V40" s="9">
+      <c r="V40" s="8">
         <v>0.0289838341151807</v>
       </c>
-      <c r="W40" s="9">
+      <c r="W40" s="8">
         <v>0.00349815603377755</v>
       </c>
-      <c r="X40" s="9">
+      <c r="X40" s="8">
         <v>0.130420097170061</v>
       </c>
     </row>
@@ -52726,16 +53297,16 @@
       <c r="S41" t="s">
         <v>190</v>
       </c>
-      <c r="U41" s="9">
+      <c r="U41" s="8">
         <v>0.0636749505817516</v>
       </c>
-      <c r="V41" s="9">
+      <c r="V41" s="8">
         <v>0.0361567135005017</v>
       </c>
-      <c r="W41" s="9">
+      <c r="W41" s="8">
         <v>0.0157348651490582</v>
       </c>
-      <c r="X41" s="9">
+      <c r="X41" s="8">
         <v>0.137843496465311</v>
       </c>
     </row>
@@ -52788,16 +53359,16 @@
       <c r="T42" t="s">
         <v>27</v>
       </c>
-      <c r="U42" s="9">
+      <c r="U42" s="8">
         <v>0.0568826779474421</v>
       </c>
-      <c r="V42" s="9">
+      <c r="V42" s="8">
         <v>0.0658017277479962</v>
       </c>
-      <c r="W42" s="9">
+      <c r="W42" s="8">
         <v>0.0191811805049551</v>
       </c>
-      <c r="X42" s="9">
+      <c r="X42" s="8">
         <v>0.130625357096033</v>
       </c>
     </row>
@@ -52850,16 +53421,16 @@
       <c r="T43" s="7" t="s">
         <v>65</v>
       </c>
-      <c r="U43" s="10">
+      <c r="U43" s="9">
         <v>0.0176870773235952</v>
       </c>
-      <c r="V43" s="10">
+      <c r="V43" s="9">
         <v>0.00776158769925157</v>
       </c>
-      <c r="W43" s="10">
+      <c r="W43" s="9">
         <v>0.0115211407343568</v>
       </c>
-      <c r="X43" s="10">
+      <c r="X43" s="9">
         <v>0.117765988083645</v>
       </c>
     </row>
@@ -52912,16 +53483,16 @@
       <c r="T44" t="s">
         <v>110</v>
       </c>
-      <c r="U44" s="9">
+      <c r="U44" s="8">
         <v>0.0344434340057601</v>
       </c>
-      <c r="V44" s="9">
+      <c r="V44" s="8">
         <v>0.00894494141414924</v>
       </c>
-      <c r="W44" s="9">
+      <c r="W44" s="8">
         <v>0.018337374185417</v>
       </c>
-      <c r="X44" s="9">
+      <c r="X44" s="8">
         <v>0.120411009125817</v>
       </c>
     </row>
@@ -52974,16 +53545,16 @@
       <c r="T45" t="s">
         <v>50</v>
       </c>
-      <c r="U45" s="9">
+      <c r="U45" s="8">
         <v>0.0246355061729748</v>
       </c>
-      <c r="V45" s="9">
+      <c r="V45" s="8">
         <v>0.0440809329350791</v>
       </c>
-      <c r="W45" s="9">
+      <c r="W45" s="8">
         <v>0.00235279401140508</v>
       </c>
-      <c r="X45" s="9">
+      <c r="X45" s="8">
         <v>0.138504411289718</v>
       </c>
     </row>
@@ -53036,16 +53607,16 @@
       <c r="T46" t="s">
         <v>100</v>
       </c>
-      <c r="U46" s="9">
+      <c r="U46" s="8">
         <v>0.0816796216964951</v>
       </c>
-      <c r="V46" s="9">
+      <c r="V46" s="8">
         <v>0.0473158846403332</v>
       </c>
-      <c r="W46" s="9">
+      <c r="W46" s="8">
         <v>0.025044104906095</v>
       </c>
-      <c r="X46" s="9">
+      <c r="X46" s="8">
         <v>0.140886008564977</v>
       </c>
     </row>
@@ -53098,16 +53669,16 @@
       <c r="T47" t="s">
         <v>279</v>
       </c>
-      <c r="U47" s="9">
+      <c r="U47" s="8">
         <v>0.0329273829976089</v>
       </c>
-      <c r="V47" s="9">
+      <c r="V47" s="8">
         <v>0.00556056806742463</v>
       </c>
-      <c r="W47" s="9">
+      <c r="W47" s="8">
         <v>0.00860160960074035</v>
       </c>
-      <c r="X47" s="9">
+      <c r="X47" s="8">
         <v>0.137396989570248</v>
       </c>
     </row>
@@ -53160,16 +53731,16 @@
       <c r="T48" t="s">
         <v>130</v>
       </c>
-      <c r="U48" s="9">
+      <c r="U48" s="8">
         <v>0.0820820376566431</v>
       </c>
-      <c r="V48" s="9">
+      <c r="V48" s="8">
         <v>0.0539090274746099</v>
       </c>
-      <c r="W48" s="9">
+      <c r="W48" s="8">
         <v>0.00772223544707924</v>
       </c>
-      <c r="X48" s="9">
+      <c r="X48" s="8">
         <v>0.139205186195313</v>
       </c>
     </row>
@@ -53222,16 +53793,16 @@
       <c r="T49" t="s">
         <v>160</v>
       </c>
-      <c r="U49" s="9">
+      <c r="U49" s="8">
         <v>0.0513259299682383</v>
       </c>
-      <c r="V49" s="9">
+      <c r="V49" s="8">
         <v>0.0181770085366066</v>
       </c>
-      <c r="W49" s="9">
+      <c r="W49" s="8">
         <v>0.0158677691225287</v>
       </c>
-      <c r="X49" s="9">
+      <c r="X49" s="8">
         <v>0.131536256916469</v>
       </c>
     </row>
@@ -53284,16 +53855,16 @@
       <c r="T50" t="s">
         <v>165</v>
       </c>
-      <c r="U50" s="9">
+      <c r="U50" s="8">
         <v>0.0369610805735827</v>
       </c>
-      <c r="V50" s="9">
+      <c r="V50" s="8">
         <v>0.0580096599765837</v>
       </c>
-      <c r="W50" s="9">
+      <c r="W50" s="8">
         <v>0.0106185453561582</v>
       </c>
-      <c r="X50" s="9">
+      <c r="X50" s="8">
         <v>0.123166941829842</v>
       </c>
     </row>
@@ -53346,16 +53917,16 @@
       <c r="T51" t="s">
         <v>175</v>
       </c>
-      <c r="U51" s="9">
+      <c r="U51" s="8">
         <v>0.0532482623240904</v>
       </c>
-      <c r="V51" s="9">
+      <c r="V51" s="8">
         <v>0.0148873419697745</v>
       </c>
-      <c r="W51" s="9">
+      <c r="W51" s="8">
         <v>0.00770280391517531</v>
       </c>
-      <c r="X51" s="9">
+      <c r="X51" s="8">
         <v>0.139591530245732</v>
       </c>
     </row>
@@ -53408,16 +53979,16 @@
       <c r="T52" t="s">
         <v>180</v>
       </c>
-      <c r="U52" s="9">
+      <c r="U52" s="8">
         <v>0.101262846725668</v>
       </c>
-      <c r="V52" s="9">
+      <c r="V52" s="8">
         <v>0.0253282343546285</v>
       </c>
-      <c r="W52" s="9">
+      <c r="W52" s="8">
         <v>0.0140355396323059</v>
       </c>
-      <c r="X52" s="9">
+      <c r="X52" s="8">
         <v>0.162598411636912</v>
       </c>
     </row>
@@ -53470,16 +54041,16 @@
       <c r="T53" t="s">
         <v>155</v>
       </c>
-      <c r="U53" s="9">
+      <c r="U53" s="8">
         <v>0.0423291899212071</v>
       </c>
-      <c r="V53" s="9">
+      <c r="V53" s="8">
         <v>0.0187454354173561</v>
       </c>
-      <c r="W53" s="9">
+      <c r="W53" s="8">
         <v>0.0201843115549306</v>
       </c>
-      <c r="X53" s="9">
+      <c r="X53" s="8">
         <v>0.139189048754946</v>
       </c>
     </row>
@@ -53532,16 +54103,16 @@
       <c r="T54" t="s">
         <v>40</v>
       </c>
-      <c r="U54" s="9">
+      <c r="U54" s="8">
         <v>0.0602768395562932</v>
       </c>
-      <c r="V54" s="9">
+      <c r="V54" s="8">
         <v>0.018685659015496</v>
       </c>
-      <c r="W54" s="9">
+      <c r="W54" s="8">
         <v>0.0177312418918557</v>
       </c>
-      <c r="X54" s="9">
+      <c r="X54" s="8">
         <v>0.137778695031416</v>
       </c>
     </row>
@@ -53594,16 +54165,16 @@
       <c r="T55" t="s">
         <v>140</v>
       </c>
-      <c r="U55" s="9">
+      <c r="U55" s="8">
         <v>0.0294362877806028</v>
       </c>
-      <c r="V55" s="9">
+      <c r="V55" s="8">
         <v>0.0121026138464623</v>
       </c>
-      <c r="W55" s="9">
+      <c r="W55" s="8">
         <v>0.000198215246200562</v>
       </c>
-      <c r="X55" s="9">
+      <c r="X55" s="8">
         <v>0.137084368527812</v>
       </c>
     </row>
@@ -53656,16 +54227,16 @@
       <c r="T56" t="s">
         <v>55</v>
       </c>
-      <c r="U56" s="9">
+      <c r="U56" s="8">
         <v>0.0227288713532219</v>
       </c>
-      <c r="V56" s="9">
+      <c r="V56" s="8">
         <v>0.0210343056442465</v>
       </c>
-      <c r="W56" s="9">
+      <c r="W56" s="8">
         <v>0.00404281715690065</v>
       </c>
-      <c r="X56" s="9">
+      <c r="X56" s="8">
         <v>0.128673008452132</v>
       </c>
     </row>
@@ -53718,16 +54289,16 @@
       <c r="T57" t="s">
         <v>120</v>
       </c>
-      <c r="U57" s="9">
+      <c r="U57" s="8">
         <v>0.0396434813737869</v>
       </c>
-      <c r="V57" s="9">
+      <c r="V57" s="8">
         <v>0.00316227475801714</v>
       </c>
-      <c r="W57" s="9">
+      <c r="W57" s="8">
         <v>0.00885361433029175</v>
       </c>
-      <c r="X57" s="9">
+      <c r="X57" s="8">
         <v>0.130156221075579</v>
       </c>
     </row>
@@ -53780,16 +54351,16 @@
       <c r="T58" t="s">
         <v>75</v>
       </c>
-      <c r="U58" s="9">
+      <c r="U58" s="8">
         <v>0.0548196572538925</v>
       </c>
-      <c r="V58" s="9">
+      <c r="V58" s="8">
         <v>0.025837854704248</v>
       </c>
-      <c r="W58" s="9">
+      <c r="W58" s="8">
         <v>0.0194550898452564</v>
       </c>
-      <c r="X58" s="9">
+      <c r="X58" s="8">
         <v>0.141295402099066</v>
       </c>
     </row>
@@ -53842,16 +54413,16 @@
       <c r="T59" t="s">
         <v>115</v>
       </c>
-      <c r="U59" s="9">
+      <c r="U59" s="8">
         <v>0.0862687577803929</v>
       </c>
-      <c r="V59" s="9">
+      <c r="V59" s="8">
         <v>0.0037595232327894</v>
       </c>
-      <c r="W59" s="9">
+      <c r="W59" s="8">
         <v>0.0209236840407074</v>
       </c>
-      <c r="X59" s="9">
+      <c r="X59" s="8">
         <v>0.120272227190701</v>
       </c>
     </row>
@@ -53904,16 +54475,16 @@
       <c r="T60" t="s">
         <v>45</v>
       </c>
-      <c r="U60" s="9">
+      <c r="U60" s="8">
         <v>0.0889766201070111</v>
       </c>
-      <c r="V60" s="9">
+      <c r="V60" s="8">
         <v>0.0142627195819429</v>
       </c>
-      <c r="W60" s="9">
+      <c r="W60" s="8">
         <v>0.00718890912063451</v>
       </c>
-      <c r="X60" s="9">
+      <c r="X60" s="8">
         <v>0.166294707165111</v>
       </c>
     </row>
@@ -53966,16 +54537,16 @@
       <c r="T61" t="s">
         <v>105</v>
       </c>
-      <c r="U61" s="9">
+      <c r="U61" s="8">
         <v>0.0410439582378903</v>
       </c>
-      <c r="V61" s="9">
+      <c r="V61" s="8">
         <v>0.0124878457274739</v>
       </c>
-      <c r="W61" s="9">
+      <c r="W61" s="8">
         <v>0.0041886439448245</v>
       </c>
-      <c r="X61" s="9">
+      <c r="X61" s="8">
         <v>0.119465989712471</v>
       </c>
     </row>
@@ -54028,16 +54599,16 @@
       <c r="T62" t="s">
         <v>170</v>
       </c>
-      <c r="U62" s="9">
+      <c r="U62" s="8">
         <v>0.0322321901718776</v>
       </c>
-      <c r="V62" s="9">
+      <c r="V62" s="8">
         <v>0.0284006347258885</v>
       </c>
-      <c r="W62" s="9">
+      <c r="W62" s="8">
         <v>0.0257180829842888</v>
       </c>
-      <c r="X62" s="9">
+      <c r="X62" s="8">
         <v>0.111648243033454</v>
       </c>
     </row>
@@ -54090,16 +54661,16 @@
       <c r="T63" t="s">
         <v>125</v>
       </c>
-      <c r="U63" s="9">
+      <c r="U63" s="8">
         <v>0.0628295232216163</v>
       </c>
-      <c r="V63" s="9">
+      <c r="V63" s="8">
         <v>0.0275812873280667</v>
       </c>
-      <c r="W63" s="9">
+      <c r="W63" s="8">
         <v>0.0176252579512254</v>
       </c>
-      <c r="X63" s="9">
+      <c r="X63" s="8">
         <v>0.128007667254592</v>
       </c>
     </row>
@@ -54152,16 +54723,16 @@
       <c r="T64" t="s">
         <v>60</v>
       </c>
-      <c r="U64" s="9">
+      <c r="U64" s="8">
         <v>0.0620914623141291</v>
       </c>
-      <c r="V64" s="9">
+      <c r="V64" s="8">
         <v>0.0110038767258349</v>
       </c>
-      <c r="W64" s="9">
+      <c r="W64" s="8">
         <v>0.00906216104825202</v>
       </c>
-      <c r="X64" s="9">
+      <c r="X64" s="8">
         <v>0.155749237220108</v>
       </c>
     </row>
@@ -54214,16 +54785,16 @@
       <c r="T65" t="s">
         <v>80</v>
       </c>
-      <c r="U65" s="9">
+      <c r="U65" s="8">
         <v>0.00265740851561461</v>
       </c>
-      <c r="V65" s="9">
+      <c r="V65" s="8">
         <v>0.00499324003856252</v>
       </c>
-      <c r="W65" s="9">
+      <c r="W65" s="8">
         <v>0.00487780570985025</v>
       </c>
-      <c r="X65" s="9">
+      <c r="X65" s="8">
         <v>0.127082200222115</v>
       </c>
     </row>
@@ -54276,16 +54847,16 @@
       <c r="T66" t="s">
         <v>90</v>
       </c>
-      <c r="U66" s="9">
+      <c r="U66" s="8">
         <v>0.0230129012206492</v>
       </c>
-      <c r="V66" s="9">
+      <c r="V66" s="8">
         <v>0.0144553748157719</v>
       </c>
-      <c r="W66" s="9">
+      <c r="W66" s="8">
         <v>0.0088042409688662</v>
       </c>
-      <c r="X66" s="9">
+      <c r="X66" s="8">
         <v>0.110791243492215</v>
       </c>
     </row>
@@ -54338,16 +54909,16 @@
       <c r="T67" t="s">
         <v>135</v>
       </c>
-      <c r="U67" s="9">
+      <c r="U67" s="8">
         <v>0.0161886685389705</v>
       </c>
-      <c r="V67" s="9">
+      <c r="V67" s="8">
         <v>0.00741761635214486</v>
       </c>
-      <c r="W67" s="9">
+      <c r="W67" s="8">
         <v>0.020803412094752</v>
       </c>
-      <c r="X67" s="9">
+      <c r="X67" s="8">
         <v>0.120998190554474</v>
       </c>
     </row>
@@ -54400,16 +54971,16 @@
       <c r="T68" t="s">
         <v>85</v>
       </c>
-      <c r="U68" s="9">
+      <c r="U68" s="8">
         <v>0.0548855913619907</v>
       </c>
-      <c r="V68" s="9">
+      <c r="V68" s="8">
         <v>0.0260503361612742</v>
       </c>
-      <c r="W68" s="9">
+      <c r="W68" s="8">
         <v>0.0176618040175498</v>
       </c>
-      <c r="X68" s="9">
+      <c r="X68" s="8">
         <v>0.146388290584783</v>
       </c>
     </row>
@@ -54462,16 +55033,16 @@
       <c r="T69" t="s">
         <v>34</v>
       </c>
-      <c r="U69" s="9">
+      <c r="U69" s="8">
         <v>0.0505920465709189</v>
       </c>
-      <c r="V69" s="9">
+      <c r="V69" s="8">
         <v>0.0176428450918949</v>
       </c>
-      <c r="W69" s="9">
+      <c r="W69" s="8">
         <v>0.00637517852179051</v>
       </c>
-      <c r="X69" s="9">
+      <c r="X69" s="8">
         <v>0.171461545113319</v>
       </c>
     </row>
@@ -54524,16 +55095,16 @@
       <c r="T70" t="s">
         <v>70</v>
       </c>
-      <c r="U70" s="9">
+      <c r="U70" s="8">
         <v>0.00317670653264359</v>
       </c>
-      <c r="V70" s="9">
+      <c r="V70" s="8">
         <v>0.0257278730471931</v>
       </c>
-      <c r="W70" s="9">
+      <c r="W70" s="8">
         <v>0.00569073359171008</v>
       </c>
-      <c r="X70" s="9">
+      <c r="X70" s="8">
         <v>0.147072413098049</v>
       </c>
     </row>
@@ -54586,16 +55157,16 @@
       <c r="T71" t="s">
         <v>145</v>
       </c>
-      <c r="U71" s="9">
+      <c r="U71" s="8">
         <v>0.0293493866920471</v>
       </c>
-      <c r="V71" s="9">
+      <c r="V71" s="8">
         <v>0.0532554388046259</v>
       </c>
-      <c r="W71" s="9">
+      <c r="W71" s="8">
         <v>0.00210356712343948</v>
       </c>
-      <c r="X71" s="9">
+      <c r="X71" s="8">
         <v>0.146614192378689</v>
       </c>
     </row>
@@ -54648,16 +55219,16 @@
       <c r="T72" t="s">
         <v>150</v>
       </c>
-      <c r="U72" s="9">
+      <c r="U72" s="8">
         <v>0.0269881226596797</v>
       </c>
-      <c r="V72" s="9">
+      <c r="V72" s="8">
         <v>0.00473445727088837</v>
       </c>
-      <c r="W72" s="9">
+      <c r="W72" s="8">
         <v>0.00664176322398638</v>
       </c>
-      <c r="X72" s="9">
+      <c r="X72" s="8">
         <v>0.154713127432186</v>
       </c>
     </row>
@@ -54710,16 +55281,16 @@
       <c r="T73" t="s">
         <v>95</v>
       </c>
-      <c r="U73" s="9">
+      <c r="U73" s="8">
         <v>0.0519193569981016</v>
       </c>
-      <c r="V73" s="9">
+      <c r="V73" s="8">
         <v>0.0338860667034805</v>
       </c>
-      <c r="W73" s="9">
+      <c r="W73" s="8">
         <v>0.00402045297343647</v>
       </c>
-      <c r="X73" s="9">
+      <c r="X73" s="8">
         <v>0.124091238937856</v>
       </c>
     </row>
@@ -54772,16 +55343,16 @@
       <c r="T74" t="s">
         <v>185</v>
       </c>
-      <c r="U74" s="9">
+      <c r="U74" s="8">
         <v>0.036981802316079</v>
       </c>
-      <c r="V74" s="9">
+      <c r="V74" s="8">
         <v>0.023601392897323</v>
       </c>
-      <c r="W74" s="9">
+      <c r="W74" s="8">
         <v>0.0191462398221993</v>
       </c>
-      <c r="X74" s="9">
+      <c r="X74" s="8">
         <v>0.144727455489849</v>
       </c>
     </row>
@@ -54834,16 +55405,16 @@
       <c r="S75" t="s">
         <v>815</v>
       </c>
-      <c r="U75" s="9">
+      <c r="U75" s="8">
         <v>0.0585123793551373</v>
       </c>
-      <c r="V75" s="9">
+      <c r="V75" s="8">
         <v>0.0439361481153401</v>
       </c>
-      <c r="W75" s="9">
+      <c r="W75" s="8">
         <v>0.0153175781583618</v>
       </c>
-      <c r="X75" s="9">
+      <c r="X75" s="8">
         <v>0.132398272575799</v>
       </c>
     </row>
@@ -55068,19 +55639,19 @@
       <c r="L81" t="s">
         <v>14</v>
       </c>
-      <c r="N81" s="9">
+      <c r="N81" s="8">
         <v>0.377898494402567</v>
       </c>
-      <c r="O81" s="9">
+      <c r="O81" s="8">
         <v>0.592570556534661</v>
       </c>
-      <c r="P81" s="9">
+      <c r="P81" s="8">
         <v>0.718069420920478</v>
       </c>
-      <c r="Q81" s="9">
+      <c r="Q81" s="8">
         <v>0.813044461939069</v>
       </c>
-      <c r="R81" s="9">
+      <c r="R81" s="8">
         <v>0.625395733449194</v>
       </c>
     </row>
@@ -55118,19 +55689,19 @@
       <c r="M82" t="s">
         <v>14</v>
       </c>
-      <c r="N82" s="9">
+      <c r="N82" s="8">
         <v>0.377898494402567</v>
       </c>
-      <c r="O82" s="9">
+      <c r="O82" s="8">
         <v>0.592570556534661</v>
       </c>
-      <c r="P82" s="9">
+      <c r="P82" s="8">
         <v>0.718069420920478</v>
       </c>
-      <c r="Q82" s="9">
+      <c r="Q82" s="8">
         <v>0.813044461939069</v>
       </c>
-      <c r="R82" s="9">
+      <c r="R82" s="8">
         <v>0.625395733449194</v>
       </c>
     </row>
@@ -55168,19 +55739,19 @@
       <c r="L83" t="s">
         <v>26</v>
       </c>
-      <c r="N83" s="9">
+      <c r="N83" s="8">
         <v>0.43497907799772</v>
       </c>
-      <c r="O83" s="9">
+      <c r="O83" s="8">
         <v>0.615422183958192</v>
       </c>
-      <c r="P83" s="9">
+      <c r="P83" s="8">
         <v>0.725662292912602</v>
       </c>
-      <c r="Q83" s="9">
+      <c r="Q83" s="8">
         <v>0.843892694968316</v>
       </c>
-      <c r="R83" s="9">
+      <c r="R83" s="8">
         <v>0.654989062459208</v>
       </c>
     </row>
@@ -55218,19 +55789,19 @@
       <c r="M84" t="s">
         <v>27</v>
       </c>
-      <c r="N84" s="9">
+      <c r="N84" s="8">
         <v>0.427502577503522</v>
       </c>
-      <c r="O84" s="9">
+      <c r="O84" s="8">
         <v>0.620487219757504</v>
       </c>
-      <c r="P84" s="9">
+      <c r="P84" s="8">
         <v>0.730520851082272</v>
       </c>
-      <c r="Q84" s="9">
+      <c r="Q84" s="8">
         <v>0.843759563234117</v>
       </c>
-      <c r="R84" s="9">
+      <c r="R84" s="8">
         <v>0.655567552894353</v>
       </c>
     </row>
@@ -55265,22 +55836,22 @@
       <c r="J85" s="1">
         <v>0.843541165192922</v>
       </c>
-      <c r="M85" s="8" t="s">
+      <c r="M85" s="3" t="s">
         <v>65</v>
       </c>
-      <c r="N85" s="10">
+      <c r="N85" s="9">
         <v>0.430719152092933</v>
       </c>
-      <c r="O85" s="10">
+      <c r="O85" s="9">
         <v>0.636071264743805</v>
       </c>
-      <c r="P85" s="10">
+      <c r="P85" s="9">
         <v>0.730298936367034</v>
       </c>
-      <c r="Q85" s="10">
+      <c r="Q85" s="9">
         <v>0.847038825352986</v>
       </c>
-      <c r="R85" s="10">
+      <c r="R85" s="9">
         <v>0.66103204463919</v>
       </c>
     </row>
@@ -55318,19 +55889,19 @@
       <c r="M86" t="s">
         <v>110</v>
       </c>
-      <c r="N86" s="9">
+      <c r="N86" s="8">
         <v>0.44649731947316</v>
       </c>
-      <c r="O86" s="9">
+      <c r="O86" s="8">
         <v>0.587737060255474</v>
       </c>
-      <c r="P86" s="9">
+      <c r="P86" s="8">
         <v>0.735317283206516</v>
       </c>
-      <c r="Q86" s="9">
+      <c r="Q86" s="8">
         <v>0.840857982635498</v>
       </c>
-      <c r="R86" s="9">
+      <c r="R86" s="8">
         <v>0.652602411392662</v>
       </c>
     </row>
@@ -55368,19 +55939,19 @@
       <c r="M87" t="s">
         <v>50</v>
       </c>
-      <c r="N87" s="9">
+      <c r="N87" s="8">
         <v>0.389022584590647</v>
       </c>
-      <c r="O87" s="9">
+      <c r="O87" s="8">
         <v>0.635782248444027</v>
       </c>
-      <c r="P87" s="9">
+      <c r="P87" s="8">
         <v>0.716540727350446</v>
       </c>
-      <c r="Q87" s="9">
+      <c r="Q87" s="8">
         <v>0.842933462725745</v>
       </c>
-      <c r="R87" s="9">
+      <c r="R87" s="8">
         <v>0.646069755777716</v>
       </c>
     </row>
@@ -55418,19 +55989,19 @@
       <c r="M88" t="s">
         <v>100</v>
       </c>
-      <c r="N88" s="9">
+      <c r="N88" s="8">
         <v>0.44594753285249</v>
       </c>
-      <c r="O88" s="9">
+      <c r="O88" s="8">
         <v>0.606551137235429</v>
       </c>
-      <c r="P88" s="9">
+      <c r="P88" s="8">
         <v>0.729037404060363</v>
       </c>
-      <c r="Q88" s="9">
+      <c r="Q88" s="8">
         <v>0.845075680149925</v>
       </c>
-      <c r="R88" s="9">
+      <c r="R88" s="8">
         <v>0.656652938574552</v>
       </c>
     </row>
@@ -55468,19 +56039,19 @@
       <c r="M89" t="s">
         <v>279</v>
       </c>
-      <c r="N89" s="9">
+      <c r="N89" s="8">
         <v>0.352468121796846</v>
       </c>
-      <c r="O89" s="9">
+      <c r="O89" s="8">
         <v>0.624565462271372</v>
       </c>
-      <c r="P89" s="9">
+      <c r="P89" s="8">
         <v>0.731961319843927</v>
       </c>
-      <c r="Q89" s="9">
+      <c r="Q89" s="8">
         <v>0.846116443475087</v>
       </c>
-      <c r="R89" s="9">
+      <c r="R89" s="8">
         <v>0.638777836846808</v>
       </c>
     </row>
@@ -55518,19 +56089,19 @@
       <c r="M90" s="5" t="s">
         <v>130</v>
       </c>
-      <c r="N90" s="11">
+      <c r="N90" s="10">
         <v>0.486529111862182</v>
       </c>
-      <c r="O90" s="11">
+      <c r="O90" s="10">
         <v>0.623385879728529</v>
       </c>
-      <c r="P90" s="11">
+      <c r="P90" s="10">
         <v>0.732632584042019</v>
       </c>
-      <c r="Q90" s="11">
+      <c r="Q90" s="10">
         <v>0.847273680898878</v>
       </c>
-      <c r="R90" s="11">
+      <c r="R90" s="10">
         <v>0.672455314132902</v>
       </c>
     </row>
@@ -55568,19 +56139,19 @@
       <c r="M91" t="s">
         <v>160</v>
       </c>
-      <c r="N91" s="9">
+      <c r="N91" s="8">
         <v>0.473770128356086</v>
       </c>
-      <c r="O91" s="9">
+      <c r="O91" s="8">
         <v>0.6072824994723</v>
       </c>
-      <c r="P91" s="9">
+      <c r="P91" s="8">
         <v>0.720555663108825</v>
       </c>
-      <c r="Q91" s="9">
+      <c r="Q91" s="8">
         <v>0.842067552937401</v>
       </c>
-      <c r="R91" s="9">
+      <c r="R91" s="8">
         <v>0.660918960968653</v>
       </c>
     </row>
@@ -55618,19 +56189,19 @@
       <c r="M92" t="s">
         <v>165</v>
       </c>
-      <c r="N92" s="9">
+      <c r="N92" s="8">
         <v>0.455988774696986</v>
       </c>
-      <c r="O92" s="9">
+      <c r="O92" s="8">
         <v>0.637030700842539</v>
       </c>
-      <c r="P92" s="9">
+      <c r="P92" s="8">
         <v>0.724065860112508</v>
       </c>
-      <c r="Q92" s="9">
+      <c r="Q92" s="8">
         <v>0.844643970330556</v>
       </c>
-      <c r="R92" s="9">
+      <c r="R92" s="8">
         <v>0.665432326495647</v>
       </c>
     </row>
@@ -55668,19 +56239,19 @@
       <c r="M93" t="s">
         <v>175</v>
       </c>
-      <c r="N93" s="9">
+      <c r="N93" s="8">
         <v>0.365320936673217</v>
       </c>
-      <c r="O93" s="9">
+      <c r="O93" s="8">
         <v>0.601111087534162</v>
       </c>
-      <c r="P93" s="9">
+      <c r="P93" s="8">
         <v>0.723296827740139</v>
       </c>
-      <c r="Q93" s="9">
+      <c r="Q93" s="8">
         <v>0.840321792496574</v>
       </c>
-      <c r="R93" s="9">
+      <c r="R93" s="8">
         <v>0.632512661111023</v>
       </c>
     </row>
@@ -55718,19 +56289,19 @@
       <c r="M94" t="s">
         <v>180</v>
       </c>
-      <c r="N94" s="9">
+      <c r="N94" s="8">
         <v>0.433622098631328</v>
       </c>
-      <c r="O94" s="9">
+      <c r="O94" s="8">
         <v>0.632566154003143</v>
       </c>
-      <c r="P94" s="9">
+      <c r="P94" s="8">
         <v>0.741636017958323</v>
       </c>
-      <c r="Q94" s="9">
+      <c r="Q94" s="8">
         <v>0.843403862582312</v>
       </c>
-      <c r="R94" s="9">
+      <c r="R94" s="8">
         <v>0.662807033293777</v>
       </c>
     </row>
@@ -55768,19 +56339,19 @@
       <c r="M95" t="s">
         <v>155</v>
       </c>
-      <c r="N95" s="9">
+      <c r="N95" s="8">
         <v>0.458568374315897</v>
       </c>
-      <c r="O95" s="9">
+      <c r="O95" s="8">
         <v>0.622160401609208</v>
       </c>
-      <c r="P95" s="9">
+      <c r="P95" s="8">
         <v>0.715844247076246</v>
       </c>
-      <c r="Q95" s="9">
+      <c r="Q95" s="8">
         <v>0.846943610244327</v>
       </c>
-      <c r="R95" s="9">
+      <c r="R95" s="8">
         <v>0.660879158311419</v>
       </c>
     </row>
@@ -55818,19 +56389,19 @@
       <c r="M96" t="s">
         <v>40</v>
       </c>
-      <c r="N96" s="9">
+      <c r="N96" s="8">
         <v>0.453887482484181</v>
       </c>
-      <c r="O96" s="9">
+      <c r="O96" s="8">
         <v>0.600814448462592</v>
       </c>
-      <c r="P96" s="9">
+      <c r="P96" s="8">
         <v>0.724232739872402</v>
       </c>
-      <c r="Q96" s="9">
+      <c r="Q96" s="8">
         <v>0.836558275752597</v>
       </c>
-      <c r="R96" s="9">
+      <c r="R96" s="8">
         <v>0.653873236642943</v>
       </c>
     </row>
@@ -55868,19 +56439,19 @@
       <c r="M97" t="s">
         <v>140</v>
       </c>
-      <c r="N97" s="9">
+      <c r="N97" s="8">
         <v>0.447806105017661</v>
       </c>
-      <c r="O97" s="9">
+      <c r="O97" s="8">
         <v>0.625932494799296</v>
       </c>
-      <c r="P97" s="9">
+      <c r="P97" s="8">
         <v>0.732123070293002</v>
       </c>
-      <c r="Q97" s="9">
+      <c r="Q97" s="8">
         <v>0.842126488685607</v>
       </c>
-      <c r="R97" s="9">
+      <c r="R97" s="8">
         <v>0.661997039698892</v>
       </c>
     </row>
@@ -55918,19 +56489,19 @@
       <c r="M98" t="s">
         <v>55</v>
       </c>
-      <c r="N98" s="9">
+      <c r="N98" s="8">
         <v>0.435851464668909</v>
       </c>
-      <c r="O98" s="9">
+      <c r="O98" s="8">
         <v>0.632115993234846</v>
       </c>
-      <c r="P98" s="9">
+      <c r="P98" s="8">
         <v>0.735183351569705</v>
       </c>
-      <c r="Q98" s="9">
+      <c r="Q98" s="8">
         <v>0.843378802140553</v>
       </c>
-      <c r="R98" s="9">
+      <c r="R98" s="8">
         <v>0.661632402903503</v>
       </c>
     </row>
@@ -55968,19 +56539,19 @@
       <c r="M99" t="s">
         <v>120</v>
       </c>
-      <c r="N99" s="9">
+      <c r="N99" s="8">
         <v>0.44820416967074</v>
       </c>
-      <c r="O99" s="9">
+      <c r="O99" s="8">
         <v>0.61500064531962</v>
       </c>
-      <c r="P99" s="9">
+      <c r="P99" s="8">
         <v>0.72423897186915</v>
       </c>
-      <c r="Q99" s="9">
+      <c r="Q99" s="8">
         <v>0.84289860063129</v>
       </c>
-      <c r="R99" s="9">
+      <c r="R99" s="8">
         <v>0.6575855968727</v>
       </c>
     </row>
@@ -56018,19 +56589,19 @@
       <c r="M100" t="s">
         <v>75</v>
       </c>
-      <c r="N100" s="9">
+      <c r="N100" s="8">
         <v>0.453569377462069</v>
       </c>
-      <c r="O100" s="9">
+      <c r="O100" s="8">
         <v>0.635703874958886</v>
       </c>
-      <c r="P100" s="9">
+      <c r="P100" s="8">
         <v>0.720161974430083</v>
       </c>
-      <c r="Q100" s="9">
+      <c r="Q100" s="8">
         <v>0.842160065968831</v>
       </c>
-      <c r="R100" s="9">
+      <c r="R100" s="8">
         <v>0.662898823204967</v>
       </c>
     </row>
@@ -56068,19 +56639,19 @@
       <c r="M101" t="s">
         <v>115</v>
       </c>
-      <c r="N101" s="9">
+      <c r="N101" s="8">
         <v>0.414620934261216</v>
       </c>
-      <c r="O101" s="9">
+      <c r="O101" s="8">
         <v>0.600095738967259</v>
       </c>
-      <c r="P101" s="9">
+      <c r="P101" s="8">
         <v>0.727582706345452</v>
       </c>
-      <c r="Q101" s="9">
+      <c r="Q101" s="8">
         <v>0.847743431727091</v>
       </c>
-      <c r="R101" s="9">
+      <c r="R101" s="8">
         <v>0.647510702825254</v>
       </c>
     </row>
@@ -56118,19 +56689,19 @@
       <c r="M102" t="s">
         <v>45</v>
       </c>
-      <c r="N102" s="9">
+      <c r="N102" s="8">
         <v>0.417204678058624</v>
       </c>
-      <c r="O102" s="9">
+      <c r="O102" s="8">
         <v>0.624122632874382</v>
       </c>
-      <c r="P102" s="9">
+      <c r="P102" s="8">
         <v>0.730794694688585</v>
       </c>
-      <c r="Q102" s="9">
+      <c r="Q102" s="8">
         <v>0.846150868468814</v>
       </c>
-      <c r="R102" s="9">
+      <c r="R102" s="8">
         <v>0.654568218522601</v>
       </c>
     </row>
@@ -56168,19 +56739,19 @@
       <c r="M103" t="s">
         <v>105</v>
       </c>
-      <c r="N103" s="9">
+      <c r="N103" s="8">
         <v>0.415641566117604</v>
       </c>
-      <c r="O103" s="9">
+      <c r="O103" s="8">
         <v>0.621664222743776</v>
       </c>
-      <c r="P103" s="9">
+      <c r="P103" s="8">
         <v>0.73826441499922</v>
       </c>
-      <c r="Q103" s="9">
+      <c r="Q103" s="8">
         <v>0.841829319794972</v>
       </c>
-      <c r="R103" s="9">
+      <c r="R103" s="8">
         <v>0.654349880913893</v>
       </c>
     </row>
@@ -56218,19 +56789,19 @@
       <c r="M104" t="s">
         <v>170</v>
       </c>
-      <c r="N104" s="9">
+      <c r="N104" s="8">
         <v>0.43862499958939</v>
       </c>
-      <c r="O104" s="9">
+      <c r="O104" s="8">
         <v>0.606166660785675</v>
       </c>
-      <c r="P104" s="9">
+      <c r="P104" s="8">
         <v>0.713780555460188</v>
       </c>
-      <c r="Q104" s="9">
+      <c r="Q104" s="8">
         <v>0.841337435775333</v>
       </c>
-      <c r="R104" s="9">
+      <c r="R104" s="8">
         <v>0.649977412902646</v>
       </c>
     </row>
@@ -56268,19 +56839,19 @@
       <c r="M105" t="s">
         <v>125</v>
       </c>
-      <c r="N105" s="9">
+      <c r="N105" s="8">
         <v>0.383867690960566</v>
       </c>
-      <c r="O105" s="9">
+      <c r="O105" s="8">
         <v>0.623502499527401</v>
       </c>
-      <c r="P105" s="9">
+      <c r="P105" s="8">
         <v>0.740728656450907</v>
       </c>
-      <c r="Q105" s="9">
+      <c r="Q105" s="8">
         <v>0.846209559175703</v>
       </c>
-      <c r="R105" s="9">
+      <c r="R105" s="8">
         <v>0.648577101528644</v>
       </c>
     </row>
@@ -56318,19 +56889,19 @@
       <c r="M106" t="s">
         <v>60</v>
       </c>
-      <c r="N106" s="9">
+      <c r="N106" s="8">
         <v>0.443450753887494</v>
       </c>
-      <c r="O106" s="9">
+      <c r="O106" s="8">
         <v>0.649935632944107</v>
       </c>
-      <c r="P106" s="9">
+      <c r="P106" s="8">
         <v>0.722174386183421</v>
       </c>
-      <c r="Q106" s="9">
+      <c r="Q106" s="8">
         <v>0.845146616299947</v>
       </c>
-      <c r="R106" s="9">
+      <c r="R106" s="8">
         <v>0.665176847328742</v>
       </c>
     </row>
@@ -56368,19 +56939,19 @@
       <c r="M107" t="s">
         <v>80</v>
       </c>
-      <c r="N107" s="9">
+      <c r="N107" s="8">
         <v>0.433006937305132</v>
       </c>
-      <c r="O107" s="9">
+      <c r="O107" s="8">
         <v>0.58378862010108</v>
       </c>
-      <c r="P107" s="9">
+      <c r="P107" s="8">
         <v>0.725821342733171</v>
       </c>
-      <c r="Q107" s="9">
+      <c r="Q107" s="8">
         <v>0.844931728310055</v>
       </c>
-      <c r="R107" s="9">
+      <c r="R107" s="8">
         <v>0.64688715711236</v>
       </c>
     </row>
@@ -56418,19 +56989,19 @@
       <c r="M108" t="s">
         <v>90</v>
       </c>
-      <c r="N108" s="9">
+      <c r="N108" s="8">
         <v>0.438855051994323</v>
       </c>
-      <c r="O108" s="9">
+      <c r="O108" s="8">
         <v>0.581090466843711</v>
       </c>
-      <c r="P108" s="9">
+      <c r="P108" s="8">
         <v>0.72642758819792</v>
       </c>
-      <c r="Q108" s="9">
+      <c r="Q108" s="8">
         <v>0.843175378110673</v>
       </c>
-      <c r="R108" s="9">
+      <c r="R108" s="8">
         <v>0.647387121286657</v>
       </c>
     </row>
@@ -56468,19 +57039,19 @@
       <c r="M109" t="s">
         <v>135</v>
       </c>
-      <c r="N109" s="9">
+      <c r="N109" s="8">
         <v>0.462766331103113</v>
       </c>
-      <c r="O109" s="9">
+      <c r="O109" s="8">
         <v>0.611778881814744</v>
       </c>
-      <c r="P109" s="9">
+      <c r="P109" s="8">
         <v>0.71422302060657</v>
       </c>
-      <c r="Q109" s="9">
+      <c r="Q109" s="8">
         <v>0.842916660838657</v>
       </c>
-      <c r="R109" s="9">
+      <c r="R109" s="8">
         <v>0.657921223590771</v>
       </c>
     </row>
@@ -56518,19 +57089,19 @@
       <c r="M110" t="s">
         <v>85</v>
       </c>
-      <c r="N110" s="9">
+      <c r="N110" s="8">
         <v>0.398638089497883</v>
       </c>
-      <c r="O110" s="9">
+      <c r="O110" s="8">
         <v>0.634552160898844</v>
       </c>
-      <c r="P110" s="9">
+      <c r="P110" s="8">
         <v>0.730238139629364</v>
       </c>
-      <c r="Q110" s="9">
+      <c r="Q110" s="8">
         <v>0.849117000897725</v>
       </c>
-      <c r="R110" s="9">
+      <c r="R110" s="8">
         <v>0.653136347730954</v>
       </c>
     </row>
@@ -56568,19 +57139,19 @@
       <c r="M111" t="s">
         <v>34</v>
       </c>
-      <c r="N111" s="9">
+      <c r="N111" s="8">
         <v>0.40298573507203</v>
       </c>
-      <c r="O111" s="9">
+      <c r="O111" s="8">
         <v>0.614381515317493</v>
       </c>
-      <c r="P111" s="9">
+      <c r="P111" s="8">
         <v>0.711603820323943</v>
       </c>
-      <c r="Q111" s="9">
+      <c r="Q111" s="8">
         <v>0.841970715257856</v>
       </c>
-      <c r="R111" s="9">
+      <c r="R111" s="8">
         <v>0.64273544649283</v>
       </c>
     </row>
@@ -56618,19 +57189,19 @@
       <c r="M112" t="s">
         <v>70</v>
       </c>
-      <c r="N112" s="9">
+      <c r="N112" s="8">
         <v>0.471682396199968</v>
       </c>
-      <c r="O112" s="9">
+      <c r="O112" s="8">
         <v>0.618915971782472</v>
       </c>
-      <c r="P112" s="9">
+      <c r="P112" s="8">
         <v>0.69936501317554</v>
       </c>
-      <c r="Q112" s="9">
+      <c r="Q112" s="8">
         <v>0.843152145544687</v>
       </c>
-      <c r="R112" s="9">
+      <c r="R112" s="8">
         <v>0.658278881675667</v>
       </c>
     </row>
@@ -56668,19 +57239,19 @@
       <c r="M113" t="s">
         <v>145</v>
       </c>
-      <c r="N113" s="9">
+      <c r="N113" s="8">
         <v>0.461749934487872</v>
       </c>
-      <c r="O113" s="9">
+      <c r="O113" s="8">
         <v>0.625313778718312</v>
       </c>
-      <c r="P113" s="9">
+      <c r="P113" s="8">
         <v>0.725269271267784</v>
       </c>
-      <c r="Q113" s="9">
+      <c r="Q113" s="8">
         <v>0.844744457138909</v>
       </c>
-      <c r="R113" s="9">
+      <c r="R113" s="8">
         <v>0.664269360403219</v>
       </c>
     </row>
@@ -56718,19 +57289,19 @@
       <c r="M114" t="s">
         <v>150</v>
       </c>
-      <c r="N114" s="9">
+      <c r="N114" s="8">
         <v>0.475100861655341</v>
       </c>
-      <c r="O114" s="9">
+      <c r="O114" s="8">
         <v>0.563845074839062</v>
       </c>
-      <c r="P114" s="9">
+      <c r="P114" s="8">
         <v>0.719201498561435</v>
       </c>
-      <c r="Q114" s="9">
+      <c r="Q114" s="8">
         <v>0.84186119503445</v>
       </c>
-      <c r="R114" s="9">
+      <c r="R114" s="8">
         <v>0.650002157522572</v>
       </c>
     </row>
@@ -56768,19 +57339,19 @@
       <c r="M115" t="s">
         <v>95</v>
       </c>
-      <c r="N115" s="9">
+      <c r="N115" s="8">
         <v>0.450946256518363</v>
       </c>
-      <c r="O115" s="9">
+      <c r="O115" s="8">
         <v>0.640044563346439</v>
       </c>
-      <c r="P115" s="9">
+      <c r="P115" s="8">
         <v>0.725301418039533</v>
       </c>
-      <c r="Q115" s="9">
+      <c r="Q115" s="8">
         <v>0.842508786254458</v>
       </c>
-      <c r="R115" s="9">
+      <c r="R115" s="8">
         <v>0.664700256039699</v>
       </c>
     </row>
@@ -56818,19 +57389,19 @@
       <c r="M116" t="s">
         <v>185</v>
       </c>
-      <c r="N116" s="9">
+      <c r="N116" s="8">
         <v>0.42221551719639</v>
       </c>
-      <c r="O116" s="9">
+      <c r="O116" s="8">
         <v>0.587190157837337</v>
       </c>
-      <c r="P116" s="9">
+      <c r="P116" s="8">
         <v>0.728836205270555</v>
       </c>
-      <c r="Q116" s="9">
+      <c r="Q116" s="8">
         <v>0.849514623483021</v>
       </c>
-      <c r="R116" s="9">
+      <c r="R116" s="8">
         <v>0.646939125946826</v>
       </c>
     </row>
@@ -56868,19 +57439,19 @@
       <c r="L117" t="s">
         <v>190</v>
       </c>
-      <c r="N117" s="9">
+      <c r="N117" s="8">
         <v>0.409652822514933</v>
       </c>
-      <c r="O117" s="9">
+      <c r="O117" s="8">
         <v>0.575478621636437</v>
       </c>
-      <c r="P117" s="9">
+      <c r="P117" s="8">
         <v>0.730191470308696</v>
       </c>
-      <c r="Q117" s="9">
+      <c r="Q117" s="8">
         <v>0.84032208173909</v>
       </c>
-      <c r="R117" s="9">
+      <c r="R117" s="8">
         <v>0.638911249049789</v>
       </c>
     </row>
@@ -56918,19 +57489,19 @@
       <c r="M118" t="s">
         <v>27</v>
       </c>
-      <c r="N118" s="9">
+      <c r="N118" s="8">
         <v>0.448997823728455</v>
       </c>
-      <c r="O118" s="9">
+      <c r="O118" s="8">
         <v>0.506620794534683</v>
       </c>
-      <c r="P118" s="9">
+      <c r="P118" s="8">
         <v>0.727595190207163</v>
       </c>
-      <c r="Q118" s="9">
+      <c r="Q118" s="8">
         <v>0.831975175274742</v>
       </c>
-      <c r="R118" s="9">
+      <c r="R118" s="8">
         <v>0.628797245936261</v>
       </c>
     </row>
@@ -56968,19 +57539,19 @@
       <c r="M119" s="7" t="s">
         <v>65</v>
       </c>
-      <c r="N119" s="10">
+      <c r="N119" s="9">
         <v>0.450348789493243</v>
       </c>
-      <c r="O119" s="10">
+      <c r="O119" s="9">
         <v>0.614285141229629</v>
       </c>
-      <c r="P119" s="10">
+      <c r="P119" s="9">
         <v>0.736019353071848</v>
       </c>
-      <c r="Q119" s="10">
+      <c r="Q119" s="9">
         <v>0.836551825205485</v>
       </c>
-      <c r="R119" s="10">
+      <c r="R119" s="9">
         <v>0.659301277250051</v>
       </c>
     </row>
@@ -57018,19 +57589,19 @@
       <c r="M120" t="s">
         <v>110</v>
       </c>
-      <c r="N120" s="9">
+      <c r="N120" s="8">
         <v>0.448615256283018</v>
       </c>
-      <c r="O120" s="9">
+      <c r="O120" s="8">
         <v>0.5855696035756</v>
       </c>
-      <c r="P120" s="9">
+      <c r="P120" s="8">
         <v>0.737939318021138</v>
       </c>
-      <c r="Q120" s="9">
+      <c r="Q120" s="8">
         <v>0.841679367754194</v>
       </c>
-      <c r="R120" s="9">
+      <c r="R120" s="8">
         <v>0.653450886408488</v>
       </c>
     </row>
@@ -57068,19 +57639,19 @@
       <c r="M121" t="s">
         <v>50</v>
       </c>
-      <c r="N121" s="9">
+      <c r="N121" s="8">
         <v>0.405255484084288</v>
       </c>
-      <c r="O121" s="9">
+      <c r="O121" s="8">
         <v>0.587015966574351</v>
       </c>
-      <c r="P121" s="9">
+      <c r="P121" s="8">
         <v>0.736374378204345</v>
       </c>
-      <c r="Q121" s="9">
+      <c r="Q121" s="8">
         <v>0.841845800479252</v>
       </c>
-      <c r="R121" s="9">
+      <c r="R121" s="8">
         <v>0.642622907335559</v>
       </c>
     </row>
@@ -57118,19 +57689,19 @@
       <c r="M122" t="s">
         <v>100</v>
       </c>
-      <c r="N122" s="9">
+      <c r="N122" s="8">
         <v>0.409294640024502</v>
       </c>
-      <c r="O122" s="9">
+      <c r="O122" s="8">
         <v>0.581136710113949</v>
       </c>
-      <c r="P122" s="9">
+      <c r="P122" s="8">
         <v>0.725142379601796</v>
       </c>
-      <c r="Q122" s="9">
+      <c r="Q122" s="8">
         <v>0.836272597312927</v>
       </c>
-      <c r="R122" s="9">
+      <c r="R122" s="8">
         <v>0.637961581763293</v>
       </c>
     </row>
@@ -57168,19 +57739,19 @@
       <c r="M123" t="s">
         <v>279</v>
       </c>
-      <c r="N123" s="9">
+      <c r="N123" s="8">
         <v>0.401890718274646</v>
       </c>
-      <c r="O123" s="9">
+      <c r="O123" s="8">
         <v>0.577795048554738</v>
       </c>
-      <c r="P123" s="9">
+      <c r="P123" s="8">
         <v>0.734710739718543</v>
       </c>
-      <c r="Q123" s="9">
+      <c r="Q123" s="8">
         <v>0.838343620300292</v>
       </c>
-      <c r="R123" s="9">
+      <c r="R123" s="8">
         <v>0.638185031712055</v>
       </c>
     </row>
@@ -57218,19 +57789,19 @@
       <c r="M124" t="s">
         <v>130</v>
       </c>
-      <c r="N124" s="9">
+      <c r="N124" s="8">
         <v>0.423057859970463</v>
       </c>
-      <c r="O124" s="9">
+      <c r="O124" s="8">
         <v>0.570805112520853</v>
       </c>
-      <c r="P124" s="9">
+      <c r="P124" s="8">
         <v>0.734154005845387</v>
       </c>
-      <c r="Q124" s="9">
+      <c r="Q124" s="8">
         <v>0.841156091954973</v>
       </c>
-      <c r="R124" s="9">
+      <c r="R124" s="8">
         <v>0.642293267572919</v>
       </c>
     </row>
@@ -57268,19 +57839,19 @@
       <c r="M125" t="s">
         <v>160</v>
       </c>
-      <c r="N125" s="9">
+      <c r="N125" s="8">
         <v>0.40676936507225</v>
       </c>
-      <c r="O125" s="9">
+      <c r="O125" s="8">
         <v>0.579197247823079</v>
       </c>
-      <c r="P125" s="9">
+      <c r="P125" s="8">
         <v>0.718226949373881</v>
       </c>
-      <c r="Q125" s="9">
+      <c r="Q125" s="8">
         <v>0.836862742900848</v>
       </c>
-      <c r="R125" s="9">
+      <c r="R125" s="8">
         <v>0.635264076292514</v>
       </c>
     </row>
@@ -57318,19 +57889,19 @@
       <c r="M126" t="s">
         <v>165</v>
       </c>
-      <c r="N126" s="9">
+      <c r="N126" s="8">
         <v>0.466597606738408</v>
       </c>
-      <c r="O126" s="9">
+      <c r="O126" s="8">
         <v>0.512084477477603</v>
       </c>
-      <c r="P126" s="9">
+      <c r="P126" s="8">
         <v>0.733159919579823</v>
       </c>
-      <c r="Q126" s="9">
+      <c r="Q126" s="8">
         <v>0.837923175758785</v>
       </c>
-      <c r="R126" s="9">
+      <c r="R126" s="8">
         <v>0.637441294888655</v>
       </c>
     </row>
@@ -57368,19 +57939,19 @@
       <c r="M127" t="s">
         <v>175</v>
       </c>
-      <c r="N127" s="9">
+      <c r="N127" s="8">
         <v>0.391278013586998</v>
       </c>
-      <c r="O127" s="9">
+      <c r="O127" s="8">
         <v>0.566416727172003</v>
       </c>
-      <c r="P127" s="9">
+      <c r="P127" s="8">
         <v>0.723809381326039</v>
       </c>
-      <c r="Q127" s="9">
+      <c r="Q127" s="8">
         <v>0.840027385287814</v>
       </c>
-      <c r="R127" s="9">
+      <c r="R127" s="8">
         <v>0.630382876843214</v>
       </c>
     </row>
@@ -57418,19 +57989,19 @@
       <c r="M128" t="s">
         <v>180</v>
       </c>
-      <c r="N128" s="9">
+      <c r="N128" s="8">
         <v>0.373690818746884</v>
       </c>
-      <c r="O128" s="9">
+      <c r="O128" s="8">
         <v>0.598366346624162</v>
       </c>
-      <c r="P128" s="9">
+      <c r="P128" s="8">
         <v>0.739945411682128</v>
       </c>
-      <c r="Q128" s="9">
+      <c r="Q128" s="8">
         <v>0.840577728218502</v>
       </c>
-      <c r="R128" s="9">
+      <c r="R128" s="8">
         <v>0.638145076317919</v>
       </c>
     </row>
@@ -57468,19 +58039,19 @@
       <c r="M129" t="s">
         <v>155</v>
       </c>
-      <c r="N129" s="9">
+      <c r="N129" s="8">
         <v>0.390456747677591</v>
       </c>
-      <c r="O129" s="9">
+      <c r="O129" s="8">
         <v>0.574035773674646</v>
       </c>
-      <c r="P129" s="9">
+      <c r="P129" s="8">
         <v>0.723242898782094</v>
       </c>
-      <c r="Q129" s="9">
+      <c r="Q129" s="8">
         <v>0.844701912668016</v>
       </c>
-      <c r="R129" s="9">
+      <c r="R129" s="8">
         <v>0.633109333200587</v>
       </c>
     </row>
@@ -57518,19 +58089,19 @@
       <c r="M130" t="s">
         <v>40</v>
       </c>
-      <c r="N130" s="9">
+      <c r="N130" s="8">
         <v>0.394262065490086</v>
       </c>
-      <c r="O130" s="9">
+      <c r="O130" s="8">
         <v>0.588308523098628</v>
       </c>
-      <c r="P130" s="9">
+      <c r="P130" s="8">
         <v>0.716535303327772</v>
       </c>
-      <c r="Q130" s="9">
+      <c r="Q130" s="8">
         <v>0.844365424580044</v>
       </c>
-      <c r="R130" s="9">
+      <c r="R130" s="8">
         <v>0.635867829124132</v>
       </c>
     </row>
@@ -57568,19 +58139,19 @@
       <c r="M131" t="s">
         <v>140</v>
       </c>
-      <c r="N131" s="9">
+      <c r="N131" s="8">
         <v>0.394954485197862</v>
       </c>
-      <c r="O131" s="9">
+      <c r="O131" s="8">
         <v>0.537858307361602</v>
       </c>
-      <c r="P131" s="9">
+      <c r="P131" s="8">
         <v>0.726654201745987</v>
       </c>
-      <c r="Q131" s="9">
+      <c r="Q131" s="8">
         <v>0.844846924146016</v>
       </c>
-      <c r="R131" s="9">
+      <c r="R131" s="8">
         <v>0.626078479612866</v>
       </c>
     </row>
@@ -57618,19 +58189,19 @@
       <c r="M132" t="s">
         <v>55</v>
       </c>
-      <c r="N132" s="9">
+      <c r="N132" s="8">
         <v>0.417543858289718</v>
       </c>
-      <c r="O132" s="9">
+      <c r="O132" s="8">
         <v>0.586360090308719</v>
       </c>
-      <c r="P132" s="9">
+      <c r="P132" s="8">
         <v>0.729258093569013</v>
       </c>
-      <c r="Q132" s="9">
+      <c r="Q132" s="8">
         <v>0.847255918714734</v>
       </c>
-      <c r="R132" s="9">
+      <c r="R132" s="8">
         <v>0.645104490220546</v>
       </c>
     </row>
@@ -57668,19 +58239,19 @@
       <c r="M133" t="s">
         <v>120</v>
       </c>
-      <c r="N133" s="9">
+      <c r="N133" s="8">
         <v>0.438655401269594</v>
       </c>
-      <c r="O133" s="9">
+      <c r="O133" s="8">
         <v>0.587828387816747</v>
       </c>
-      <c r="P133" s="9">
+      <c r="P133" s="8">
         <v>0.752100567022959</v>
       </c>
-      <c r="Q133" s="9">
+      <c r="Q133" s="8">
         <v>0.835289706786473</v>
       </c>
-      <c r="R133" s="9">
+      <c r="R133" s="8">
         <v>0.653468515723943</v>
       </c>
     </row>
@@ -57718,19 +58289,19 @@
       <c r="M134" t="s">
         <v>75</v>
       </c>
-      <c r="N134" s="9">
+      <c r="N134" s="8">
         <v>0.391705313490496</v>
       </c>
-      <c r="O134" s="9">
+      <c r="O134" s="8">
         <v>0.576453778478834</v>
       </c>
-      <c r="P134" s="9">
+      <c r="P134" s="8">
         <v>0.725251323646969</v>
       </c>
-      <c r="Q134" s="9">
+      <c r="Q134" s="8">
         <v>0.838920182651943</v>
       </c>
-      <c r="R134" s="9">
+      <c r="R134" s="8">
         <v>0.633082649567061</v>
       </c>
     </row>
@@ -57768,19 +58339,19 @@
       <c r="M135" t="s">
         <v>115</v>
       </c>
-      <c r="N135" s="9">
+      <c r="N135" s="8">
         <v>0.461305643121401</v>
       </c>
-      <c r="O135" s="9">
+      <c r="O135" s="8">
         <v>0.561619083086649</v>
       </c>
-      <c r="P135" s="9">
+      <c r="P135" s="8">
         <v>0.725251744190852</v>
       </c>
-      <c r="Q135" s="9">
+      <c r="Q135" s="8">
         <v>0.835261811812719</v>
       </c>
-      <c r="R135" s="9">
+      <c r="R135" s="8">
         <v>0.645859570552905</v>
       </c>
     </row>
@@ -57818,19 +58389,19 @@
       <c r="M136" t="s">
         <v>45</v>
       </c>
-      <c r="N136" s="9">
+      <c r="N136" s="8">
         <v>0.353485505614015</v>
       </c>
-      <c r="O136" s="9">
+      <c r="O136" s="8">
         <v>0.594011988904741</v>
       </c>
-      <c r="P136" s="9">
+      <c r="P136" s="8">
         <v>0.736036803987291</v>
       </c>
-      <c r="Q136" s="9">
+      <c r="Q136" s="8">
         <v>0.841857247882419</v>
       </c>
-      <c r="R136" s="9">
+      <c r="R136" s="8">
         <v>0.631347886597116</v>
       </c>
     </row>
@@ -57868,19 +58439,19 @@
       <c r="M137" t="s">
         <v>105</v>
       </c>
-      <c r="N137" s="9">
+      <c r="N137" s="8">
         <v>0.446316993898815</v>
       </c>
-      <c r="O137" s="9">
+      <c r="O137" s="8">
         <v>0.580909470717112</v>
       </c>
-      <c r="P137" s="9">
+      <c r="P137" s="8">
         <v>0.732362071673075</v>
       </c>
-      <c r="Q137" s="9">
+      <c r="Q137" s="8">
         <v>0.844140728314717</v>
       </c>
-      <c r="R137" s="9">
+      <c r="R137" s="8">
         <v>0.65093231615093</v>
       </c>
     </row>
@@ -57918,19 +58489,19 @@
       <c r="M138" t="s">
         <v>170</v>
       </c>
-      <c r="N138" s="9">
+      <c r="N138" s="8">
         <v>0.46712105969588</v>
       </c>
-      <c r="O138" s="9">
+      <c r="O138" s="8">
         <v>0.591120466589928</v>
       </c>
-      <c r="P138" s="9">
+      <c r="P138" s="8">
         <v>0.731115072965622</v>
       </c>
-      <c r="Q138" s="9">
+      <c r="Q138" s="8">
         <v>0.84021171927452</v>
       </c>
-      <c r="R138" s="9">
+      <c r="R138" s="8">
         <v>0.657392079631487</v>
       </c>
     </row>
@@ -57968,19 +58539,19 @@
       <c r="M139" t="s">
         <v>125</v>
       </c>
-      <c r="N139" s="9">
+      <c r="N139" s="8">
         <v>0.433799963858392</v>
       </c>
-      <c r="O139" s="9">
+      <c r="O139" s="8">
         <v>0.59250052107705</v>
       </c>
-      <c r="P139" s="9">
+      <c r="P139" s="8">
         <v>0.73067965110143</v>
       </c>
-      <c r="Q139" s="9">
+      <c r="Q139" s="8">
         <v>0.840284095870123</v>
       </c>
-      <c r="R139" s="9">
+      <c r="R139" s="8">
         <v>0.649316057976749</v>
       </c>
     </row>
@@ -58018,19 +58589,19 @@
       <c r="M140" t="s">
         <v>60</v>
       </c>
-      <c r="N140" s="9">
+      <c r="N140" s="8">
         <v>0.372132169703642</v>
       </c>
-      <c r="O140" s="9">
+      <c r="O140" s="8">
         <v>0.575136388341585</v>
       </c>
-      <c r="P140" s="9">
+      <c r="P140" s="8">
         <v>0.742268492778142</v>
       </c>
-      <c r="Q140" s="9">
+      <c r="Q140" s="8">
         <v>0.844386865695318</v>
       </c>
-      <c r="R140" s="9">
+      <c r="R140" s="8">
         <v>0.633480979129672</v>
       </c>
     </row>
@@ -58068,19 +58639,19 @@
       <c r="M141" t="s">
         <v>80</v>
       </c>
-      <c r="N141" s="9">
+      <c r="N141" s="8">
         <v>0.411940500140189</v>
       </c>
-      <c r="O141" s="9">
+      <c r="O141" s="8">
         <v>0.593438684940338</v>
       </c>
-      <c r="P141" s="9">
+      <c r="P141" s="8">
         <v>0.721515119075775</v>
       </c>
-      <c r="Q141" s="9">
+      <c r="Q141" s="8">
         <v>0.837438156207402</v>
       </c>
-      <c r="R141" s="9">
+      <c r="R141" s="8">
         <v>0.641083115090926</v>
       </c>
     </row>
@@ -58118,19 +58689,19 @@
       <c r="M142" t="s">
         <v>90</v>
       </c>
-      <c r="N142" s="9">
+      <c r="N142" s="8">
         <v>0.466502027379142</v>
       </c>
-      <c r="O142" s="9">
+      <c r="O142" s="8">
         <v>0.570507023069593</v>
       </c>
-      <c r="P142" s="9">
+      <c r="P142" s="8">
         <v>0.732745673921372</v>
       </c>
-      <c r="Q142" s="9">
+      <c r="Q142" s="8">
         <v>0.838307824399736</v>
       </c>
-      <c r="R142" s="9">
+      <c r="R142" s="8">
         <v>0.652015637192461</v>
       </c>
     </row>
@@ -58168,19 +58739,19 @@
       <c r="M143" t="s">
         <v>135</v>
       </c>
-      <c r="N143" s="9">
+      <c r="N143" s="8">
         <v>0.444504886865615</v>
       </c>
-      <c r="O143" s="9">
+      <c r="O143" s="8">
         <v>0.569037460618548</v>
       </c>
-      <c r="P143" s="9">
+      <c r="P143" s="8">
         <v>0.737262917889489</v>
       </c>
-      <c r="Q143" s="9">
+      <c r="Q143" s="8">
         <v>0.835396488507588</v>
       </c>
-      <c r="R143" s="9">
+      <c r="R143" s="8">
         <v>0.64655043847031</v>
       </c>
     </row>
@@ -58218,19 +58789,19 @@
       <c r="M144" t="s">
         <v>85</v>
       </c>
-      <c r="N144" s="9">
+      <c r="N144" s="8">
         <v>0.385453833474053</v>
       </c>
-      <c r="O144" s="9">
+      <c r="O144" s="8">
         <v>0.579962114493051</v>
       </c>
-      <c r="P144" s="9">
+      <c r="P144" s="8">
         <v>0.731812987062666</v>
       </c>
-      <c r="Q144" s="9">
+      <c r="Q144" s="8">
         <v>0.841909964879353</v>
       </c>
-      <c r="R144" s="9">
+      <c r="R144" s="8">
         <v>0.634784724977281</v>
       </c>
     </row>
@@ -58268,19 +58839,19 @@
       <c r="M145" t="s">
         <v>34</v>
       </c>
-      <c r="N145" s="9">
+      <c r="N145" s="8">
         <v>0.323111393799384</v>
       </c>
-      <c r="O145" s="9">
+      <c r="O145" s="8">
         <v>0.599495616224077</v>
       </c>
-      <c r="P145" s="9">
+      <c r="P145" s="8">
         <v>0.727080470985836</v>
       </c>
-      <c r="Q145" s="9">
+      <c r="Q145" s="8">
         <v>0.840097056494818</v>
       </c>
-      <c r="R145" s="9">
+      <c r="R145" s="8">
         <v>0.622446134376029</v>
       </c>
     </row>
@@ -58318,19 +58889,19 @@
       <c r="M146" t="s">
         <v>70</v>
       </c>
-      <c r="N146" s="9">
+      <c r="N146" s="8">
         <v>0.37088917940855</v>
       </c>
-      <c r="O146" s="9">
+      <c r="O146" s="8">
         <v>0.587736343344052</v>
       </c>
-      <c r="P146" s="9">
+      <c r="P146" s="8">
         <v>0.726320266723633</v>
       </c>
-      <c r="Q146" s="9">
+      <c r="Q146" s="8">
         <v>0.838348696629206</v>
       </c>
-      <c r="R146" s="9">
+      <c r="R146" s="8">
         <v>0.63082362152636</v>
       </c>
     </row>
@@ -58368,19 +58939,19 @@
       <c r="M147" t="s">
         <v>145</v>
       </c>
-      <c r="N147" s="9">
+      <c r="N147" s="8">
         <v>0.372567921876907</v>
       </c>
-      <c r="O147" s="9">
+      <c r="O147" s="8">
         <v>0.553266644477844</v>
       </c>
-      <c r="P147" s="9">
+      <c r="P147" s="8">
         <v>0.721159021059672</v>
       </c>
-      <c r="Q147" s="9">
+      <c r="Q147" s="8">
         <v>0.846244891484578</v>
       </c>
-      <c r="R147" s="9">
+      <c r="R147" s="8">
         <v>0.62330961972475</v>
       </c>
     </row>
@@ -58418,19 +58989,19 @@
       <c r="M148" t="s">
         <v>150</v>
       </c>
-      <c r="N148" s="9">
+      <c r="N148" s="8">
         <v>0.361297118994924</v>
       </c>
-      <c r="O148" s="9">
+      <c r="O148" s="8">
         <v>0.575616078244315</v>
       </c>
-      <c r="P148" s="9">
+      <c r="P148" s="8">
         <v>0.736916820208231</v>
       </c>
-      <c r="Q148" s="9">
+      <c r="Q148" s="8">
         <v>0.843750185436672</v>
       </c>
-      <c r="R148" s="9">
+      <c r="R148" s="8">
         <v>0.629395050721035</v>
       </c>
     </row>
@@ -58468,19 +59039,19 @@
       <c r="M149" t="s">
         <v>95</v>
       </c>
-      <c r="N149" s="9">
+      <c r="N149" s="8">
         <v>0.435151038898362</v>
       </c>
-      <c r="O149" s="9">
+      <c r="O149" s="8">
         <v>0.580191390381919</v>
       </c>
-      <c r="P149" s="9">
+      <c r="P149" s="8">
         <v>0.726134618123372</v>
       </c>
-      <c r="Q149" s="9">
+      <c r="Q149" s="8">
         <v>0.841371887260013</v>
       </c>
-      <c r="R149" s="9">
+      <c r="R149" s="8">
         <v>0.645712233665916</v>
       </c>
     </row>
@@ -58518,19 +59089,19 @@
       <c r="M150" t="s">
         <v>185</v>
       </c>
-      <c r="N150" s="9">
+      <c r="N150" s="8">
         <v>0.375803795125749</v>
       </c>
-      <c r="O150" s="9">
+      <c r="O150" s="8">
         <v>0.56761360168457</v>
       </c>
-      <c r="P150" s="9">
+      <c r="P150" s="8">
         <v>0.72315854496426</v>
       </c>
-      <c r="Q150" s="9">
+      <c r="Q150" s="8">
         <v>0.84209402402242</v>
       </c>
-      <c r="R150" s="9">
+      <c r="R150" s="8">
         <v>0.62716749144925</v>
       </c>
     </row>
@@ -58568,19 +59139,19 @@
       <c r="L151" t="s">
         <v>815</v>
       </c>
-      <c r="N151" s="9">
+      <c r="N151" s="8">
         <v>0.42207866050435</v>
       </c>
-      <c r="O151" s="9">
+      <c r="O151" s="8">
         <v>0.596148077953369</v>
       </c>
-      <c r="P151" s="9">
+      <c r="P151" s="8">
         <v>0.72768526191407</v>
       </c>
-      <c r="Q151" s="9">
+      <c r="Q151" s="8">
         <v>0.841710092433801</v>
       </c>
-      <c r="R151" s="9">
+      <c r="R151" s="8">
         <v>0.646905523201397</v>
       </c>
     </row>

</xml_diff>